<commit_message>
commit tesouro para venda sem grafico
</commit_message>
<xml_diff>
--- a/TESOURO DIRETO_0519 - Venda.xlsx
+++ b/TESOURO DIRETO_0519 - Venda.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="020519" sheetId="21" r:id="rId1"/>
     <sheet name="030519" sheetId="22" r:id="rId2"/>
     <sheet name="060519" sheetId="23" r:id="rId3"/>
-    <sheet name="COMPARAÇÃO DIA A DIA" sheetId="4" r:id="rId4"/>
-    <sheet name="TESOURO IPCA" sheetId="5" r:id="rId5"/>
-    <sheet name="TESOURO IPCA JUROS SEMESTRAIS" sheetId="6" r:id="rId6"/>
-    <sheet name="TESOURO PREFIXADOS" sheetId="7" r:id="rId7"/>
-    <sheet name="TESOURO PREFIXADOS JUROS SEM." sheetId="25" r:id="rId8"/>
-    <sheet name="TESOURO SELIC" sheetId="8" r:id="rId9"/>
-    <sheet name="TESOURO IGP-M" sheetId="26" r:id="rId10"/>
+    <sheet name="070519" sheetId="27" r:id="rId4"/>
+    <sheet name="COMPARAÇÃO DIA A DIA" sheetId="4" r:id="rId5"/>
+    <sheet name="TESOURO IPCA" sheetId="5" r:id="rId6"/>
+    <sheet name="TESOURO IPCA JUROS SEMESTRAIS" sheetId="6" r:id="rId7"/>
+    <sheet name="TESOURO PREFIXADOS" sheetId="7" r:id="rId8"/>
+    <sheet name="TESOURO PREFIXADOS JUROS SEM." sheetId="25" r:id="rId9"/>
+    <sheet name="TESOURO SELIC" sheetId="8" r:id="rId10"/>
+    <sheet name="TESOURO IGP-M" sheetId="26" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -3462,9 +3463,471 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG100"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
+      <c r="Y1" s="74"/>
+      <c r="Z1" s="74"/>
+      <c r="AA1" s="74"/>
+      <c r="AB1" s="74"/>
+      <c r="AC1" s="74"/>
+      <c r="AD1" s="74"/>
+      <c r="AE1" s="74"/>
+      <c r="AF1" s="75"/>
+    </row>
+    <row r="2" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="V2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="W2" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y2" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA2" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE2" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF2" s="34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="4">
+        <v>43587</v>
+      </c>
+      <c r="D3" s="5">
+        <v>43587</v>
+      </c>
+      <c r="E3" s="3">
+        <v>43588</v>
+      </c>
+      <c r="F3" s="5">
+        <v>43588</v>
+      </c>
+      <c r="G3" s="3">
+        <v>43591</v>
+      </c>
+      <c r="H3" s="4">
+        <v>43591</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="26"/>
+      <c r="V3" s="28"/>
+      <c r="W3" s="26"/>
+      <c r="X3" s="28"/>
+      <c r="Y3" s="26"/>
+      <c r="Z3" s="28"/>
+      <c r="AA3" s="26"/>
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="26"/>
+      <c r="AD3" s="28"/>
+      <c r="AE3" s="26"/>
+      <c r="AF3" s="28"/>
+    </row>
+    <row r="4" spans="1:33" s="115" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="88" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="89">
+        <v>44256</v>
+      </c>
+      <c r="C4" s="92">
+        <v>0.01</v>
+      </c>
+      <c r="D4" s="93">
+        <v>10085.08</v>
+      </c>
+      <c r="E4" s="92">
+        <v>0.01</v>
+      </c>
+      <c r="F4" s="93">
+        <v>10087.57</v>
+      </c>
+      <c r="G4" s="92">
+        <v>0.01</v>
+      </c>
+      <c r="H4" s="93">
+        <v>10090.049999999999</v>
+      </c>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="28"/>
+      <c r="V4" s="26"/>
+      <c r="W4" s="28"/>
+      <c r="X4" s="26"/>
+      <c r="Y4" s="28"/>
+      <c r="Z4" s="26"/>
+      <c r="AA4" s="28"/>
+      <c r="AB4" s="26"/>
+      <c r="AC4" s="27"/>
+      <c r="AD4" s="26"/>
+      <c r="AE4" s="28"/>
+      <c r="AF4" s="26"/>
+      <c r="AG4" s="28"/>
+    </row>
+    <row r="5" spans="1:33" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="97" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="98">
+        <v>44986</v>
+      </c>
+      <c r="C5" s="84">
+        <v>0.02</v>
+      </c>
+      <c r="D5" s="85">
+        <v>10079.219999999999</v>
+      </c>
+      <c r="E5" s="84">
+        <v>0.02</v>
+      </c>
+      <c r="F5" s="85">
+        <v>10081.700000000001</v>
+      </c>
+      <c r="G5" s="84">
+        <v>0.02</v>
+      </c>
+      <c r="H5" s="85">
+        <v>10084.19</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="80"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="80"/>
+      <c r="R5" s="39"/>
+      <c r="S5" s="81"/>
+      <c r="T5" s="80"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="80"/>
+      <c r="W5" s="81"/>
+      <c r="X5" s="80"/>
+      <c r="Y5" s="81"/>
+      <c r="Z5" s="80"/>
+      <c r="AA5" s="81"/>
+      <c r="AB5" s="80"/>
+      <c r="AC5" s="39"/>
+      <c r="AD5" s="80"/>
+      <c r="AE5" s="81"/>
+      <c r="AF5" s="80"/>
+      <c r="AG5" s="81"/>
+    </row>
+    <row r="6" spans="1:33" s="116" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="91">
+        <v>45717</v>
+      </c>
+      <c r="C6" s="86">
+        <v>0.03</v>
+      </c>
+      <c r="D6" s="87">
+        <v>10069.31</v>
+      </c>
+      <c r="E6" s="86">
+        <v>0.03</v>
+      </c>
+      <c r="F6" s="87">
+        <v>10071.799999999999</v>
+      </c>
+      <c r="G6" s="86">
+        <v>0.03</v>
+      </c>
+      <c r="H6" s="87">
+        <v>10074.290000000001</v>
+      </c>
+      <c r="I6" s="112"/>
+      <c r="J6" s="113"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="14"/>
+      <c r="AC6" s="15"/>
+      <c r="AD6" s="14"/>
+      <c r="AE6" s="16"/>
+      <c r="AF6" s="14"/>
+      <c r="AG6" s="16"/>
+    </row>
+    <row r="7" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:AF1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
+  <pageSetup orientation="landscape"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -4473,8 +4936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5048,12 +5511,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AG115"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A36" sqref="A36:H37"/>
     </sheetView>
   </sheetViews>
@@ -7032,7 +7507,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF101"/>
   <sheetViews>
@@ -7558,7 +8033,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF103"/>
   <sheetViews>
@@ -8167,7 +8642,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG102"/>
   <sheetViews>
@@ -8627,570 +9102,6 @@
       <c r="AE8" s="81"/>
       <c r="AF8" s="80"/>
       <c r="AG8" s="81"/>
-    </row>
-    <row r="9" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:AF1"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG102"/>
-  <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="28.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="28.85546875" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="78" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="78"/>
-    </row>
-    <row r="2" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="N2" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="P2" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q2" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="R2" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="S2" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="T2" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="U2" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="V2" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="W2" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="X2" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y2" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z2" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA2" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB2" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC2" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD2" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE2" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF2" s="24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="4">
-        <v>43587</v>
-      </c>
-      <c r="D3" s="5">
-        <v>43587</v>
-      </c>
-      <c r="E3" s="3">
-        <v>43588</v>
-      </c>
-      <c r="F3" s="5">
-        <v>43588</v>
-      </c>
-      <c r="G3" s="3">
-        <v>43591</v>
-      </c>
-      <c r="H3" s="4">
-        <v>43591</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="26"/>
-      <c r="V3" s="28"/>
-      <c r="W3" s="26"/>
-      <c r="X3" s="28"/>
-      <c r="Y3" s="26"/>
-      <c r="Z3" s="28"/>
-      <c r="AA3" s="26"/>
-      <c r="AB3" s="28"/>
-      <c r="AC3" s="26"/>
-      <c r="AD3" s="28"/>
-      <c r="AE3" s="26"/>
-      <c r="AF3" s="28"/>
-    </row>
-    <row r="4" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="88" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="89">
-        <v>44197</v>
-      </c>
-      <c r="C4" s="92">
-        <v>7.19</v>
-      </c>
-      <c r="D4" s="93">
-        <v>1073.81</v>
-      </c>
-      <c r="E4" s="92">
-        <v>7.13</v>
-      </c>
-      <c r="F4" s="93">
-        <v>1075.03</v>
-      </c>
-      <c r="G4" s="92">
-        <v>7.09</v>
-      </c>
-      <c r="H4" s="93">
-        <v>1075.94</v>
-      </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="80"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="80"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="80"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="81"/>
-      <c r="T4" s="80"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="80"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="80"/>
-      <c r="Y4" s="81"/>
-      <c r="Z4" s="80"/>
-      <c r="AA4" s="81"/>
-      <c r="AB4" s="80"/>
-      <c r="AC4" s="39"/>
-      <c r="AD4" s="80"/>
-      <c r="AE4" s="81"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="81"/>
-    </row>
-    <row r="5" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="97" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="98">
-        <v>44927</v>
-      </c>
-      <c r="C5" s="84">
-        <v>8.24</v>
-      </c>
-      <c r="D5" s="85">
-        <v>1085.18</v>
-      </c>
-      <c r="E5" s="84">
-        <v>8.18</v>
-      </c>
-      <c r="F5" s="85">
-        <v>1087.3800000000001</v>
-      </c>
-      <c r="G5" s="84">
-        <v>8.1300000000000008</v>
-      </c>
-      <c r="H5" s="85">
-        <v>1089.27</v>
-      </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="80"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="80"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="80"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="80"/>
-      <c r="R5" s="39"/>
-      <c r="S5" s="81"/>
-      <c r="T5" s="80"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="80"/>
-      <c r="W5" s="81"/>
-      <c r="X5" s="80"/>
-      <c r="Y5" s="81"/>
-      <c r="Z5" s="80"/>
-      <c r="AA5" s="81"/>
-      <c r="AB5" s="80"/>
-      <c r="AC5" s="39"/>
-      <c r="AD5" s="80"/>
-      <c r="AE5" s="81"/>
-      <c r="AF5" s="80"/>
-      <c r="AG5" s="81"/>
-    </row>
-    <row r="6" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="97" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="98">
-        <v>45658</v>
-      </c>
-      <c r="C6" s="84">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="D6" s="85">
-        <v>1087.92</v>
-      </c>
-      <c r="E6" s="84">
-        <v>8.66</v>
-      </c>
-      <c r="F6" s="85">
-        <v>1090.04</v>
-      </c>
-      <c r="G6" s="84">
-        <v>8.61</v>
-      </c>
-      <c r="H6" s="85">
-        <v>1092.5899999999999</v>
-      </c>
-      <c r="I6" s="105"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="20"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="20"/>
-      <c r="V6" s="19"/>
-      <c r="W6" s="20"/>
-      <c r="X6" s="19"/>
-      <c r="Y6" s="20"/>
-      <c r="Z6" s="19"/>
-      <c r="AA6" s="20"/>
-      <c r="AB6" s="19"/>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="19"/>
-      <c r="AE6" s="20"/>
-      <c r="AF6" s="19"/>
-      <c r="AG6" s="20"/>
-    </row>
-    <row r="7" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="97" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="98">
-        <v>46388</v>
-      </c>
-      <c r="C7" s="84">
-        <v>8.99</v>
-      </c>
-      <c r="D7" s="85">
-        <v>1086.21</v>
-      </c>
-      <c r="E7" s="84">
-        <v>8.93</v>
-      </c>
-      <c r="F7" s="85">
-        <v>1089.8499999999999</v>
-      </c>
-      <c r="G7" s="84">
-        <v>8.8800000000000008</v>
-      </c>
-      <c r="H7" s="85">
-        <v>1092.96</v>
-      </c>
-      <c r="I7" s="105"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="20"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="20"/>
-      <c r="V7" s="19"/>
-      <c r="W7" s="20"/>
-      <c r="X7" s="19"/>
-      <c r="Y7" s="20"/>
-      <c r="Z7" s="19"/>
-      <c r="AA7" s="20"/>
-      <c r="AB7" s="19"/>
-      <c r="AC7" s="11"/>
-      <c r="AD7" s="19"/>
-      <c r="AE7" s="20"/>
-      <c r="AF7" s="19"/>
-      <c r="AG7" s="20"/>
-    </row>
-    <row r="8" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="90" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="91">
-        <v>47119</v>
-      </c>
-      <c r="C8" s="86">
-        <v>9.08</v>
-      </c>
-      <c r="D8" s="87">
-        <v>1090.1400000000001</v>
-      </c>
-      <c r="E8" s="86">
-        <v>9.0299999999999994</v>
-      </c>
-      <c r="F8" s="87">
-        <v>1093.69</v>
-      </c>
-      <c r="G8" s="86">
-        <v>8.99</v>
-      </c>
-      <c r="H8" s="87">
-        <v>1096.6199999999999</v>
-      </c>
-      <c r="I8" s="105"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="20"/>
-      <c r="V8" s="19"/>
-      <c r="W8" s="20"/>
-      <c r="X8" s="19"/>
-      <c r="Y8" s="20"/>
-      <c r="Z8" s="19"/>
-      <c r="AA8" s="20"/>
-      <c r="AB8" s="19"/>
-      <c r="AC8" s="11"/>
-      <c r="AD8" s="19"/>
-      <c r="AE8" s="20"/>
-      <c r="AF8" s="19"/>
-      <c r="AG8" s="20"/>
     </row>
     <row r="9" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9297,15 +9208,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG100"/>
+  <dimension ref="A1:AG102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="40" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
@@ -9320,76 +9231,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
-      <c r="U1" s="74"/>
-      <c r="V1" s="74"/>
-      <c r="W1" s="74"/>
-      <c r="X1" s="74"/>
-      <c r="Y1" s="74"/>
-      <c r="Z1" s="74"/>
-      <c r="AA1" s="74"/>
-      <c r="AB1" s="74"/>
-      <c r="AC1" s="74"/>
-      <c r="AD1" s="74"/>
-      <c r="AE1" s="74"/>
-      <c r="AF1" s="75"/>
+      <c r="A1" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
     </row>
     <row r="2" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="34" t="s">
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="33" t="s">
         <v>4</v>
       </c>
       <c r="M2" s="34" t="s">
@@ -9440,16 +9351,16 @@
       <c r="AB2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="AC2" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD2" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE2" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF2" s="34" t="s">
+      <c r="AC2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE2" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF2" s="24" t="s">
         <v>4</v>
       </c>
     </row>
@@ -9477,7 +9388,7 @@
         <v>43591</v>
       </c>
       <c r="I3" s="3"/>
-      <c r="J3" s="5"/>
+      <c r="J3" s="4"/>
       <c r="K3" s="26"/>
       <c r="L3" s="28"/>
       <c r="M3" s="26"/>
@@ -9501,81 +9412,81 @@
       <c r="AE3" s="26"/>
       <c r="AF3" s="28"/>
     </row>
-    <row r="4" spans="1:33" s="115" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="88" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B4" s="89">
-        <v>44256</v>
+        <v>44197</v>
       </c>
       <c r="C4" s="92">
-        <v>0.01</v>
+        <v>7.19</v>
       </c>
       <c r="D4" s="93">
-        <v>10085.08</v>
+        <v>1073.81</v>
       </c>
       <c r="E4" s="92">
-        <v>0.01</v>
+        <v>7.13</v>
       </c>
       <c r="F4" s="93">
-        <v>10087.57</v>
+        <v>1075.03</v>
       </c>
       <c r="G4" s="92">
-        <v>0.01</v>
+        <v>7.09</v>
       </c>
       <c r="H4" s="93">
-        <v>10090.049999999999</v>
-      </c>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="26"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="26"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="28"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="28"/>
-      <c r="V4" s="26"/>
-      <c r="W4" s="28"/>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="28"/>
-      <c r="Z4" s="26"/>
-      <c r="AA4" s="28"/>
-      <c r="AB4" s="26"/>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="26"/>
-      <c r="AE4" s="28"/>
-      <c r="AF4" s="26"/>
-      <c r="AG4" s="28"/>
-    </row>
-    <row r="5" spans="1:33" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1075.94</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="80"/>
+      <c r="R4" s="39"/>
+      <c r="S4" s="81"/>
+      <c r="T4" s="80"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="80"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="80"/>
+      <c r="Y4" s="81"/>
+      <c r="Z4" s="80"/>
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="80"/>
+      <c r="AC4" s="39"/>
+      <c r="AD4" s="80"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="81"/>
+    </row>
+    <row r="5" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="97" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B5" s="98">
-        <v>44986</v>
+        <v>44927</v>
       </c>
       <c r="C5" s="84">
-        <v>0.02</v>
+        <v>8.24</v>
       </c>
       <c r="D5" s="85">
-        <v>10079.219999999999</v>
+        <v>1085.18</v>
       </c>
       <c r="E5" s="84">
-        <v>0.02</v>
+        <v>8.18</v>
       </c>
       <c r="F5" s="85">
-        <v>10081.700000000001</v>
+        <v>1087.3800000000001</v>
       </c>
       <c r="G5" s="84">
-        <v>0.02</v>
+        <v>8.1300000000000008</v>
       </c>
       <c r="H5" s="85">
-        <v>10084.19</v>
+        <v>1089.27</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -9603,59 +9514,159 @@
       <c r="AF5" s="80"/>
       <c r="AG5" s="81"/>
     </row>
-    <row r="6" spans="1:33" s="116" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="90" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="91">
-        <v>45717</v>
-      </c>
-      <c r="C6" s="86">
-        <v>0.03</v>
-      </c>
-      <c r="D6" s="87">
-        <v>10069.31</v>
-      </c>
-      <c r="E6" s="86">
-        <v>0.03</v>
-      </c>
-      <c r="F6" s="87">
-        <v>10071.799999999999</v>
-      </c>
-      <c r="G6" s="86">
-        <v>0.03</v>
-      </c>
-      <c r="H6" s="87">
-        <v>10074.290000000001</v>
-      </c>
-      <c r="I6" s="112"/>
-      <c r="J6" s="113"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="14"/>
-      <c r="W6" s="16"/>
-      <c r="X6" s="14"/>
-      <c r="Y6" s="16"/>
-      <c r="Z6" s="14"/>
-      <c r="AA6" s="16"/>
-      <c r="AB6" s="14"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="14"/>
-      <c r="AE6" s="16"/>
-      <c r="AF6" s="14"/>
-      <c r="AG6" s="16"/>
-    </row>
-    <row r="7" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="97" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="98">
+        <v>45658</v>
+      </c>
+      <c r="C6" s="84">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D6" s="85">
+        <v>1087.92</v>
+      </c>
+      <c r="E6" s="84">
+        <v>8.66</v>
+      </c>
+      <c r="F6" s="85">
+        <v>1090.04</v>
+      </c>
+      <c r="G6" s="84">
+        <v>8.61</v>
+      </c>
+      <c r="H6" s="85">
+        <v>1092.5899999999999</v>
+      </c>
+      <c r="I6" s="105"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="20"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="20"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="20"/>
+      <c r="AB6" s="19"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="19"/>
+      <c r="AE6" s="20"/>
+      <c r="AF6" s="19"/>
+      <c r="AG6" s="20"/>
+    </row>
+    <row r="7" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="97" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="98">
+        <v>46388</v>
+      </c>
+      <c r="C7" s="84">
+        <v>8.99</v>
+      </c>
+      <c r="D7" s="85">
+        <v>1086.21</v>
+      </c>
+      <c r="E7" s="84">
+        <v>8.93</v>
+      </c>
+      <c r="F7" s="85">
+        <v>1089.8499999999999</v>
+      </c>
+      <c r="G7" s="84">
+        <v>8.8800000000000008</v>
+      </c>
+      <c r="H7" s="85">
+        <v>1092.96</v>
+      </c>
+      <c r="I7" s="105"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="20"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="20"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="20"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="19"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="19"/>
+      <c r="AE7" s="20"/>
+      <c r="AF7" s="19"/>
+      <c r="AG7" s="20"/>
+    </row>
+    <row r="8" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="90" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="91">
+        <v>47119</v>
+      </c>
+      <c r="C8" s="86">
+        <v>9.08</v>
+      </c>
+      <c r="D8" s="87">
+        <v>1090.1400000000001</v>
+      </c>
+      <c r="E8" s="86">
+        <v>9.0299999999999994</v>
+      </c>
+      <c r="F8" s="87">
+        <v>1093.69</v>
+      </c>
+      <c r="G8" s="86">
+        <v>8.99</v>
+      </c>
+      <c r="H8" s="87">
+        <v>1096.6199999999999</v>
+      </c>
+      <c r="I8" s="105"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="19"/>
+      <c r="Y8" s="20"/>
+      <c r="Z8" s="19"/>
+      <c r="AA8" s="20"/>
+      <c r="AB8" s="19"/>
+      <c r="AC8" s="11"/>
+      <c r="AD8" s="19"/>
+      <c r="AE8" s="20"/>
+      <c r="AF8" s="19"/>
+      <c r="AG8" s="20"/>
+    </row>
     <row r="9" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9748,6 +9759,8 @@
     <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:AF1"/>

</xml_diff>

<commit_message>
commit atualizacao tesouro dia 08/05
</commit_message>
<xml_diff>
--- a/TESOURO DIRETO_0519 - Venda.xlsx
+++ b/TESOURO DIRETO_0519 - Venda.xlsx
@@ -9,27 +9,28 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" firstSheet="8" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="020519" sheetId="21" r:id="rId1"/>
     <sheet name="030519" sheetId="22" r:id="rId2"/>
     <sheet name="060519" sheetId="23" r:id="rId3"/>
     <sheet name="070519" sheetId="27" r:id="rId4"/>
-    <sheet name="COMPARAÇÃO DIA A DIA" sheetId="4" r:id="rId5"/>
-    <sheet name="TESOURO IPCA" sheetId="5" r:id="rId6"/>
-    <sheet name="TESOURO IPCA JUROS SEMESTRAIS" sheetId="6" r:id="rId7"/>
-    <sheet name="TESOURO PREFIXADOS" sheetId="7" r:id="rId8"/>
-    <sheet name="TESOURO PREFIXADOS JUROS SEM." sheetId="25" r:id="rId9"/>
-    <sheet name="TESOURO SELIC" sheetId="8" r:id="rId10"/>
-    <sheet name="TESOURO IGP-M" sheetId="26" r:id="rId11"/>
+    <sheet name="080519" sheetId="28" r:id="rId5"/>
+    <sheet name="COMPARAÇÃO DIA A DIA" sheetId="4" r:id="rId6"/>
+    <sheet name="TESOURO IPCA" sheetId="5" r:id="rId7"/>
+    <sheet name="TESOURO IPCA JUROS SEMESTRAIS" sheetId="6" r:id="rId8"/>
+    <sheet name="TESOURO PREFIXADOS" sheetId="7" r:id="rId9"/>
+    <sheet name="TESOURO PREFIXADOS JUROS SEM." sheetId="25" r:id="rId10"/>
+    <sheet name="TESOURO SELIC" sheetId="8" r:id="rId11"/>
+    <sheet name="TESOURO IGP-M" sheetId="26" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="41">
   <si>
     <t>Vencimento</t>
   </si>
@@ -824,7 +825,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1078,6 +1079,49 @@
     <xf numFmtId="8" fontId="2" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1117,6 +1161,9 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1129,64 +1176,21 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="2" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="2" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="2" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="2" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1431,6 +1435,12 @@
                   <c:pt idx="7">
                     <c:v>07/05</c:v>
                   </c:pt>
+                  <c:pt idx="8">
+                    <c:v>08/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>08/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1556,6 +1566,12 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1594.93</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>4.49</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1597.97</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1688,6 +1704,12 @@
                   <c:pt idx="7">
                     <c:v>07/05</c:v>
                   </c:pt>
+                  <c:pt idx="8">
+                    <c:v>08/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>08/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -1813,6 +1835,12 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1028.27</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>4.49</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1031.22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1945,6 +1973,12 @@
                   <c:pt idx="7">
                     <c:v>07/05</c:v>
                   </c:pt>
+                  <c:pt idx="8">
+                    <c:v>08/mai</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>08/mai</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
@@ -2059,11 +2093,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-516945584"/>
-        <c:axId val="-516946672"/>
+        <c:axId val="-747765408"/>
+        <c:axId val="-747769760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-516945584"/>
+        <c:axId val="-747765408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2106,7 +2140,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-516946672"/>
+        <c:crossAx val="-747769760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2114,7 +2148,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-516946672"/>
+        <c:axId val="-747769760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2124,7 +2158,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-516945584"/>
+        <c:crossAx val="-747765408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3063,12 +3097,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="89"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="104"/>
     </row>
     <row r="2" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
@@ -3225,12 +3259,12 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="90" t="s">
+      <c r="A13" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="91"/>
-      <c r="C13" s="91"/>
-      <c r="D13" s="92"/>
+      <c r="B13" s="106"/>
+      <c r="C13" s="106"/>
+      <c r="D13" s="107"/>
     </row>
     <row r="14" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="39" t="s">
@@ -3387,12 +3421,12 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="90" t="s">
+      <c r="A25" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="91"/>
-      <c r="C25" s="91"/>
-      <c r="D25" s="92"/>
+      <c r="B25" s="106"/>
+      <c r="C25" s="106"/>
+      <c r="D25" s="107"/>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="39" t="s">
@@ -3451,12 +3485,12 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="90" t="s">
+      <c r="A30" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="91"/>
-      <c r="C30" s="91"/>
-      <c r="D30" s="92"/>
+      <c r="B30" s="106"/>
+      <c r="C30" s="106"/>
+      <c r="D30" s="107"/>
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="39" t="s">
@@ -3513,15 +3547,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG100"/>
+  <dimension ref="A1:AG102"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="40" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
@@ -3536,76 +3570,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="100" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="101"/>
-      <c r="N1" s="101"/>
-      <c r="O1" s="101"/>
-      <c r="P1" s="101"/>
-      <c r="Q1" s="101"/>
-      <c r="R1" s="101"/>
-      <c r="S1" s="101"/>
-      <c r="T1" s="101"/>
-      <c r="U1" s="101"/>
-      <c r="V1" s="101"/>
-      <c r="W1" s="101"/>
-      <c r="X1" s="101"/>
-      <c r="Y1" s="101"/>
-      <c r="Z1" s="101"/>
-      <c r="AA1" s="101"/>
-      <c r="AB1" s="101"/>
-      <c r="AC1" s="101"/>
-      <c r="AD1" s="101"/>
-      <c r="AE1" s="101"/>
-      <c r="AF1" s="102"/>
+      <c r="A1" s="124" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="124"/>
+      <c r="K1" s="124"/>
+      <c r="L1" s="124"/>
+      <c r="M1" s="124"/>
+      <c r="N1" s="124"/>
+      <c r="O1" s="124"/>
+      <c r="P1" s="124"/>
+      <c r="Q1" s="124"/>
+      <c r="R1" s="124"/>
+      <c r="S1" s="124"/>
+      <c r="T1" s="124"/>
+      <c r="U1" s="124"/>
+      <c r="V1" s="124"/>
+      <c r="W1" s="124"/>
+      <c r="X1" s="124"/>
+      <c r="Y1" s="124"/>
+      <c r="Z1" s="124"/>
+      <c r="AA1" s="124"/>
+      <c r="AB1" s="124"/>
+      <c r="AC1" s="124"/>
+      <c r="AD1" s="124"/>
+      <c r="AE1" s="124"/>
+      <c r="AF1" s="124"/>
     </row>
     <row r="2" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="30" t="s">
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="29" t="s">
         <v>4</v>
       </c>
       <c r="M2" s="30" t="s">
@@ -3656,16 +3690,16 @@
       <c r="AB2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="AC2" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD2" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF2" s="30" t="s">
+      <c r="AC2" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF2" s="21" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3698,8 +3732,12 @@
       <c r="J3" s="4">
         <v>43592</v>
       </c>
-      <c r="K3" s="22"/>
-      <c r="L3" s="24"/>
+      <c r="K3" s="22">
+        <v>43593</v>
+      </c>
+      <c r="L3" s="24">
+        <v>43593</v>
+      </c>
       <c r="M3" s="22"/>
       <c r="N3" s="24"/>
       <c r="O3" s="22"/>
@@ -3721,6 +3759,618 @@
       <c r="AE3" s="22"/>
       <c r="AF3" s="24"/>
     </row>
+    <row r="4" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="65">
+        <v>44197</v>
+      </c>
+      <c r="C4" s="68">
+        <v>7.19</v>
+      </c>
+      <c r="D4" s="69">
+        <v>1073.81</v>
+      </c>
+      <c r="E4" s="68">
+        <v>7.13</v>
+      </c>
+      <c r="F4" s="69">
+        <v>1075.03</v>
+      </c>
+      <c r="G4" s="68">
+        <v>7.09</v>
+      </c>
+      <c r="H4" s="69">
+        <v>1075.94</v>
+      </c>
+      <c r="I4" s="94">
+        <v>7.06</v>
+      </c>
+      <c r="J4" s="95">
+        <v>1076.69</v>
+      </c>
+      <c r="K4" s="94">
+        <v>7.04</v>
+      </c>
+      <c r="L4" s="95">
+        <v>1077.29</v>
+      </c>
+      <c r="M4" s="56"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="56"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="56"/>
+      <c r="R4" s="35"/>
+      <c r="S4" s="57"/>
+      <c r="T4" s="56"/>
+      <c r="U4" s="57"/>
+      <c r="V4" s="56"/>
+      <c r="W4" s="57"/>
+      <c r="X4" s="56"/>
+      <c r="Y4" s="57"/>
+      <c r="Z4" s="56"/>
+      <c r="AA4" s="57"/>
+      <c r="AB4" s="56"/>
+      <c r="AC4" s="35"/>
+      <c r="AD4" s="56"/>
+      <c r="AE4" s="57"/>
+      <c r="AF4" s="56"/>
+      <c r="AG4" s="57"/>
+    </row>
+    <row r="5" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="72">
+        <v>44927</v>
+      </c>
+      <c r="C5" s="60">
+        <v>8.24</v>
+      </c>
+      <c r="D5" s="61">
+        <v>1085.18</v>
+      </c>
+      <c r="E5" s="60">
+        <v>8.18</v>
+      </c>
+      <c r="F5" s="61">
+        <v>1087.3800000000001</v>
+      </c>
+      <c r="G5" s="60">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="H5" s="61">
+        <v>1089.27</v>
+      </c>
+      <c r="I5" s="96">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="J5" s="97">
+        <v>1089.92</v>
+      </c>
+      <c r="K5" s="96">
+        <v>8.1</v>
+      </c>
+      <c r="L5" s="97">
+        <v>1090.8800000000001</v>
+      </c>
+      <c r="M5" s="56"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="56"/>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="56"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="57"/>
+      <c r="T5" s="56"/>
+      <c r="U5" s="57"/>
+      <c r="V5" s="56"/>
+      <c r="W5" s="57"/>
+      <c r="X5" s="56"/>
+      <c r="Y5" s="57"/>
+      <c r="Z5" s="56"/>
+      <c r="AA5" s="57"/>
+      <c r="AB5" s="56"/>
+      <c r="AC5" s="35"/>
+      <c r="AD5" s="56"/>
+      <c r="AE5" s="57"/>
+      <c r="AF5" s="56"/>
+      <c r="AG5" s="57"/>
+    </row>
+    <row r="6" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="71" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="72">
+        <v>45658</v>
+      </c>
+      <c r="C6" s="60">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D6" s="61">
+        <v>1087.92</v>
+      </c>
+      <c r="E6" s="60">
+        <v>8.66</v>
+      </c>
+      <c r="F6" s="61">
+        <v>1090.04</v>
+      </c>
+      <c r="G6" s="60">
+        <v>8.61</v>
+      </c>
+      <c r="H6" s="61">
+        <v>1092.5899999999999</v>
+      </c>
+      <c r="I6" s="96">
+        <v>8.59</v>
+      </c>
+      <c r="J6" s="97">
+        <v>1093.83</v>
+      </c>
+      <c r="K6" s="96">
+        <v>8.56</v>
+      </c>
+      <c r="L6" s="97">
+        <v>1095.51</v>
+      </c>
+      <c r="M6" s="16"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="17"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="16"/>
+      <c r="AE6" s="17"/>
+      <c r="AF6" s="16"/>
+      <c r="AG6" s="17"/>
+    </row>
+    <row r="7" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="71" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="72">
+        <v>46388</v>
+      </c>
+      <c r="C7" s="60">
+        <v>8.99</v>
+      </c>
+      <c r="D7" s="61">
+        <v>1086.21</v>
+      </c>
+      <c r="E7" s="60">
+        <v>8.93</v>
+      </c>
+      <c r="F7" s="61">
+        <v>1089.8499999999999</v>
+      </c>
+      <c r="G7" s="60">
+        <v>8.8800000000000008</v>
+      </c>
+      <c r="H7" s="61">
+        <v>1092.96</v>
+      </c>
+      <c r="I7" s="96">
+        <v>8.85</v>
+      </c>
+      <c r="J7" s="97">
+        <v>1094.97</v>
+      </c>
+      <c r="K7" s="96">
+        <v>8.82</v>
+      </c>
+      <c r="L7" s="97">
+        <v>1096.99</v>
+      </c>
+      <c r="M7" s="16"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="17"/>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="17"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="16"/>
+      <c r="AE7" s="17"/>
+      <c r="AF7" s="16"/>
+      <c r="AG7" s="17"/>
+    </row>
+    <row r="8" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="66" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="67">
+        <v>47119</v>
+      </c>
+      <c r="C8" s="62">
+        <v>9.08</v>
+      </c>
+      <c r="D8" s="63">
+        <v>1090.1400000000001</v>
+      </c>
+      <c r="E8" s="62">
+        <v>9.0299999999999994</v>
+      </c>
+      <c r="F8" s="63">
+        <v>1093.69</v>
+      </c>
+      <c r="G8" s="62">
+        <v>8.99</v>
+      </c>
+      <c r="H8" s="63">
+        <v>1096.6199999999999</v>
+      </c>
+      <c r="I8" s="98">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="J8" s="99">
+        <v>1099.56</v>
+      </c>
+      <c r="K8" s="98">
+        <v>8.92</v>
+      </c>
+      <c r="L8" s="99">
+        <v>1101.8599999999999</v>
+      </c>
+      <c r="M8" s="16"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="16"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="16"/>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="16"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="16"/>
+      <c r="AE8" s="17"/>
+      <c r="AF8" s="16"/>
+      <c r="AG8" s="17"/>
+    </row>
+    <row r="9" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:AF1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
+  <pageSetup orientation="landscape"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG100"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="116" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
+      <c r="K1" s="117"/>
+      <c r="L1" s="117"/>
+      <c r="M1" s="117"/>
+      <c r="N1" s="117"/>
+      <c r="O1" s="117"/>
+      <c r="P1" s="117"/>
+      <c r="Q1" s="117"/>
+      <c r="R1" s="117"/>
+      <c r="S1" s="117"/>
+      <c r="T1" s="117"/>
+      <c r="U1" s="117"/>
+      <c r="V1" s="117"/>
+      <c r="W1" s="117"/>
+      <c r="X1" s="117"/>
+      <c r="Y1" s="117"/>
+      <c r="Z1" s="117"/>
+      <c r="AA1" s="117"/>
+      <c r="AB1" s="117"/>
+      <c r="AC1" s="117"/>
+      <c r="AD1" s="117"/>
+      <c r="AE1" s="117"/>
+      <c r="AF1" s="118"/>
+    </row>
+    <row r="2" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="V2" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="W2" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y2" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA2" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE2" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF2" s="30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="4">
+        <v>43587</v>
+      </c>
+      <c r="D3" s="5">
+        <v>43587</v>
+      </c>
+      <c r="E3" s="3">
+        <v>43588</v>
+      </c>
+      <c r="F3" s="5">
+        <v>43588</v>
+      </c>
+      <c r="G3" s="3">
+        <v>43591</v>
+      </c>
+      <c r="H3" s="4">
+        <v>43591</v>
+      </c>
+      <c r="I3" s="3">
+        <v>43592</v>
+      </c>
+      <c r="J3" s="4">
+        <v>43592</v>
+      </c>
+      <c r="K3" s="22">
+        <v>43593</v>
+      </c>
+      <c r="L3" s="24">
+        <v>43593</v>
+      </c>
+      <c r="M3" s="22"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="24"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="22"/>
+      <c r="Z3" s="24"/>
+      <c r="AA3" s="22"/>
+      <c r="AB3" s="24"/>
+      <c r="AC3" s="22"/>
+      <c r="AD3" s="24"/>
+      <c r="AE3" s="22"/>
+      <c r="AF3" s="24"/>
+    </row>
     <row r="4" spans="1:33" s="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="64" t="s">
         <v>35</v>
@@ -3746,14 +4396,18 @@
       <c r="H4" s="69">
         <v>10090.049999999999</v>
       </c>
-      <c r="I4" s="113">
+      <c r="I4" s="94">
         <v>0.01</v>
       </c>
-      <c r="J4" s="114">
+      <c r="J4" s="95">
         <v>10092.549999999999</v>
       </c>
-      <c r="K4" s="22"/>
-      <c r="L4" s="24"/>
+      <c r="K4" s="94">
+        <v>0.01</v>
+      </c>
+      <c r="L4" s="95">
+        <v>10095.030000000001</v>
+      </c>
       <c r="M4" s="22"/>
       <c r="N4" s="24"/>
       <c r="O4" s="22"/>
@@ -3801,14 +4455,18 @@
       <c r="H5" s="61">
         <v>10084.19</v>
       </c>
-      <c r="I5" s="115">
+      <c r="I5" s="96">
         <v>0.02</v>
       </c>
-      <c r="J5" s="116">
+      <c r="J5" s="97">
         <v>10086.68</v>
       </c>
-      <c r="K5" s="56"/>
-      <c r="L5" s="57"/>
+      <c r="K5" s="96">
+        <v>0.02</v>
+      </c>
+      <c r="L5" s="97">
+        <v>10089.18</v>
+      </c>
       <c r="M5" s="56"/>
       <c r="N5" s="57"/>
       <c r="O5" s="56"/>
@@ -3856,14 +4514,18 @@
       <c r="H6" s="63">
         <v>10074.290000000001</v>
       </c>
-      <c r="I6" s="117">
+      <c r="I6" s="98">
         <v>0.03</v>
       </c>
-      <c r="J6" s="118">
+      <c r="J6" s="99">
         <v>10076.780000000001</v>
       </c>
-      <c r="K6" s="11"/>
-      <c r="L6" s="13"/>
+      <c r="K6" s="98">
+        <v>0.03</v>
+      </c>
+      <c r="L6" s="99">
+        <v>10079.27</v>
+      </c>
       <c r="M6" s="11"/>
       <c r="N6" s="13"/>
       <c r="O6" s="11"/>
@@ -3989,12 +4651,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="K3" sqref="K3:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4014,40 +4676,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="116" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="101"/>
-      <c r="N1" s="101"/>
-      <c r="O1" s="101"/>
-      <c r="P1" s="101"/>
-      <c r="Q1" s="101"/>
-      <c r="R1" s="101"/>
-      <c r="S1" s="101"/>
-      <c r="T1" s="101"/>
-      <c r="U1" s="101"/>
-      <c r="V1" s="101"/>
-      <c r="W1" s="101"/>
-      <c r="X1" s="101"/>
-      <c r="Y1" s="101"/>
-      <c r="Z1" s="101"/>
-      <c r="AA1" s="101"/>
-      <c r="AB1" s="101"/>
-      <c r="AC1" s="101"/>
-      <c r="AD1" s="101"/>
-      <c r="AE1" s="101"/>
-      <c r="AF1" s="102"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
+      <c r="K1" s="117"/>
+      <c r="L1" s="117"/>
+      <c r="M1" s="117"/>
+      <c r="N1" s="117"/>
+      <c r="O1" s="117"/>
+      <c r="P1" s="117"/>
+      <c r="Q1" s="117"/>
+      <c r="R1" s="117"/>
+      <c r="S1" s="117"/>
+      <c r="T1" s="117"/>
+      <c r="U1" s="117"/>
+      <c r="V1" s="117"/>
+      <c r="W1" s="117"/>
+      <c r="X1" s="117"/>
+      <c r="Y1" s="117"/>
+      <c r="Z1" s="117"/>
+      <c r="AA1" s="117"/>
+      <c r="AB1" s="117"/>
+      <c r="AC1" s="117"/>
+      <c r="AD1" s="117"/>
+      <c r="AE1" s="117"/>
+      <c r="AF1" s="118"/>
     </row>
     <row r="2" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
@@ -4176,8 +4838,12 @@
       <c r="J3" s="15">
         <v>43592</v>
       </c>
-      <c r="K3" s="22"/>
-      <c r="L3" s="24"/>
+      <c r="K3" s="10">
+        <v>43593</v>
+      </c>
+      <c r="L3" s="15">
+        <v>43593</v>
+      </c>
       <c r="M3" s="22"/>
       <c r="N3" s="24"/>
       <c r="O3" s="22"/>
@@ -4224,14 +4890,18 @@
       <c r="H4" s="69">
         <v>4204.09</v>
       </c>
-      <c r="I4" s="113">
+      <c r="I4" s="94">
         <v>3.05</v>
       </c>
-      <c r="J4" s="114">
+      <c r="J4" s="95">
         <v>4205.83</v>
       </c>
-      <c r="K4" s="56"/>
-      <c r="L4" s="57"/>
+      <c r="K4" s="94">
+        <v>3.06</v>
+      </c>
+      <c r="L4" s="95">
+        <v>4206.08</v>
+      </c>
       <c r="M4" s="56"/>
       <c r="N4" s="57"/>
       <c r="O4" s="56"/>
@@ -4278,14 +4948,18 @@
       <c r="H5" s="63">
         <v>6827.13</v>
       </c>
-      <c r="I5" s="117">
+      <c r="I5" s="98">
         <v>4.2699999999999996</v>
       </c>
-      <c r="J5" s="118">
+      <c r="J5" s="99">
         <v>6834.05</v>
       </c>
-      <c r="K5" s="11"/>
-      <c r="L5" s="13"/>
+      <c r="K5" s="98">
+        <v>4.26</v>
+      </c>
+      <c r="L5" s="99">
+        <v>6840.97</v>
+      </c>
       <c r="M5" s="11"/>
       <c r="N5" s="13"/>
       <c r="O5" s="11"/>
@@ -4315,7 +4989,7 @@
     <row r="11" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I13" s="123"/>
+      <c r="I13" s="101"/>
     </row>
     <row r="14" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4454,12 +5128,12 @@
       <c r="I1" s="53"/>
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
+      <c r="B2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
       <c r="E2" s="36" t="s">
         <v>19</v>
       </c>
@@ -4677,12 +5351,12 @@
       <c r="I12" s="37"/>
     </row>
     <row r="13" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="96" t="s">
+      <c r="A13" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="97"/>
-      <c r="C13" s="97"/>
-      <c r="D13" s="98"/>
+      <c r="B13" s="112"/>
+      <c r="C13" s="112"/>
+      <c r="D13" s="113"/>
       <c r="E13" s="37"/>
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
@@ -4880,12 +5554,12 @@
       <c r="I23" s="53"/>
     </row>
     <row r="24" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="93" t="s">
+      <c r="A24" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="94"/>
-      <c r="C24" s="94"/>
-      <c r="D24" s="95"/>
+      <c r="B24" s="109"/>
+      <c r="C24" s="109"/>
+      <c r="D24" s="110"/>
       <c r="E24" s="37"/>
       <c r="F24" s="37"/>
       <c r="G24" s="37"/>
@@ -4950,12 +5624,12 @@
       <c r="I27" s="53"/>
     </row>
     <row r="28" spans="1:9" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="96" t="s">
+      <c r="A28" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="97"/>
-      <c r="C28" s="97"/>
-      <c r="D28" s="98"/>
+      <c r="B28" s="112"/>
+      <c r="C28" s="112"/>
+      <c r="D28" s="113"/>
       <c r="E28" s="37"/>
       <c r="F28" s="37"/>
       <c r="G28" s="37"/>
@@ -5052,12 +5726,12 @@
       <c r="I1" s="36"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="114" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
+      <c r="B2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
       <c r="E2" s="36" t="s">
         <v>19</v>
       </c>
@@ -5271,12 +5945,12 @@
       <c r="I12" s="37"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="96" t="s">
+      <c r="A13" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="97"/>
-      <c r="C13" s="97"/>
-      <c r="D13" s="98"/>
+      <c r="B13" s="112"/>
+      <c r="C13" s="112"/>
+      <c r="D13" s="113"/>
       <c r="E13" s="37"/>
       <c r="F13" s="37"/>
       <c r="G13" s="37"/>
@@ -5465,12 +6139,12 @@
       <c r="H23" s="37"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="96" t="s">
+      <c r="A24" s="111" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="97"/>
-      <c r="C24" s="97"/>
-      <c r="D24" s="98"/>
+      <c r="B24" s="112"/>
+      <c r="C24" s="112"/>
+      <c r="D24" s="113"/>
       <c r="E24" s="37"/>
       <c r="F24" s="37"/>
       <c r="G24" s="37"/>
@@ -5531,12 +6205,12 @@
       <c r="H27" s="37"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="96" t="s">
+      <c r="A28" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="97"/>
-      <c r="C28" s="97"/>
-      <c r="D28" s="98"/>
+      <c r="B28" s="112"/>
+      <c r="C28" s="112"/>
+      <c r="D28" s="113"/>
       <c r="E28" s="37"/>
       <c r="F28" s="37"/>
       <c r="G28" s="37"/>
@@ -5607,398 +6281,398 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="106" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="106" t="s">
+      <c r="C1" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="87" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-      <c r="D2" s="108"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
     </row>
     <row r="3" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="109" t="s">
+      <c r="A3" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="110">
+      <c r="B3" s="91">
         <v>43600</v>
       </c>
-      <c r="C3" s="111">
+      <c r="C3" s="92">
         <v>-1.38</v>
       </c>
-      <c r="D3" s="112">
+      <c r="D3" s="93">
         <v>3222.48</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="109" t="s">
+      <c r="A4" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="110">
+      <c r="B4" s="91">
         <v>45519</v>
       </c>
-      <c r="C4" s="111">
+      <c r="C4" s="92">
         <v>4.16</v>
       </c>
-      <c r="D4" s="112">
+      <c r="D4" s="93">
         <v>2599.7399999999998</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="109" t="s">
+      <c r="A5" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="110">
+      <c r="B5" s="91">
         <v>49444</v>
       </c>
-      <c r="C5" s="111">
+      <c r="C5" s="92">
         <v>4.5</v>
       </c>
-      <c r="D5" s="112">
+      <c r="D5" s="93">
         <v>1594.93</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="110">
+      <c r="B6" s="91">
         <v>53097</v>
       </c>
-      <c r="C6" s="111">
+      <c r="C6" s="92">
         <v>4.5</v>
       </c>
-      <c r="D6" s="112">
+      <c r="D6" s="93">
         <v>1028.27</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="109" t="s">
+      <c r="A7" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="110">
+      <c r="B7" s="91">
         <v>44058</v>
       </c>
-      <c r="C7" s="111">
+      <c r="C7" s="92">
         <v>2.82</v>
       </c>
-      <c r="D7" s="112">
+      <c r="D7" s="93">
         <v>3388.37</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="109" t="s">
+      <c r="A8" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="110">
+      <c r="B8" s="91">
         <v>45519</v>
       </c>
-      <c r="C8" s="111">
+      <c r="C8" s="92">
         <v>4.09</v>
       </c>
-      <c r="D8" s="112">
+      <c r="D8" s="93">
         <v>3548.22</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="109" t="s">
+      <c r="A9" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="110">
+      <c r="B9" s="91">
         <v>46249</v>
       </c>
-      <c r="C9" s="111">
+      <c r="C9" s="92">
         <v>4.1900000000000004</v>
       </c>
-      <c r="D9" s="112">
+      <c r="D9" s="93">
         <v>3619.29</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="109" t="s">
+      <c r="A10" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="110">
+      <c r="B10" s="91">
         <v>49444</v>
       </c>
-      <c r="C10" s="111">
+      <c r="C10" s="92">
         <v>4.41</v>
       </c>
-      <c r="D10" s="112">
+      <c r="D10" s="93">
         <v>3888.93</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="109" t="s">
+      <c r="A11" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="110">
+      <c r="B11" s="91">
         <v>53097</v>
       </c>
-      <c r="C11" s="111">
+      <c r="C11" s="92">
         <v>4.53</v>
       </c>
-      <c r="D11" s="112">
+      <c r="D11" s="93">
         <v>4024.53</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="109" t="s">
+      <c r="A12" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="110">
+      <c r="B12" s="91">
         <v>55015</v>
       </c>
-      <c r="C12" s="111">
+      <c r="C12" s="92">
         <v>4.53</v>
       </c>
-      <c r="D12" s="112">
+      <c r="D12" s="93">
         <v>4044.5</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="107" t="s">
+      <c r="A13" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="108"/>
-      <c r="C13" s="108"/>
-      <c r="D13" s="108"/>
+      <c r="B13" s="115"/>
+      <c r="C13" s="115"/>
+      <c r="D13" s="115"/>
     </row>
     <row r="14" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="109" t="s">
+      <c r="A14" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="110">
+      <c r="B14" s="91">
         <v>43831</v>
       </c>
-      <c r="C14" s="111">
+      <c r="C14" s="92">
         <v>6.48</v>
       </c>
-      <c r="D14" s="112">
+      <c r="D14" s="93">
         <v>959.24</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="109" t="s">
+      <c r="A15" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="110">
+      <c r="B15" s="91">
         <v>44197</v>
       </c>
-      <c r="C15" s="111">
+      <c r="C15" s="92">
         <v>7.11</v>
       </c>
-      <c r="D15" s="112">
+      <c r="D15" s="93">
         <v>892.31</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="109" t="s">
+      <c r="A16" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="110">
+      <c r="B16" s="91">
         <v>44562</v>
       </c>
-      <c r="C16" s="111">
+      <c r="C16" s="92">
         <v>7.79</v>
       </c>
-      <c r="D16" s="112">
+      <c r="D16" s="93">
         <v>819.43</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="109" t="s">
+      <c r="A17" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="110">
+      <c r="B17" s="91">
         <v>44927</v>
       </c>
-      <c r="C17" s="111">
+      <c r="C17" s="92">
         <v>8.25</v>
       </c>
-      <c r="D17" s="112">
+      <c r="D17" s="93">
         <v>748.7</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="109" t="s">
+      <c r="A18" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="110">
+      <c r="B18" s="91">
         <v>45658</v>
       </c>
-      <c r="C18" s="111">
+      <c r="C18" s="92">
         <v>8.77</v>
       </c>
-      <c r="D18" s="112">
+      <c r="D18" s="93">
         <v>622.07000000000005</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="109" t="s">
+      <c r="A19" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="110">
+      <c r="B19" s="91">
         <v>44197</v>
       </c>
-      <c r="C19" s="111">
+      <c r="C19" s="92">
         <v>7.06</v>
       </c>
-      <c r="D19" s="112">
+      <c r="D19" s="93">
         <v>1076.69</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="109" t="s">
+      <c r="A20" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="110">
+      <c r="B20" s="91">
         <v>44927</v>
       </c>
-      <c r="C20" s="111">
+      <c r="C20" s="92">
         <v>8.1199999999999992</v>
       </c>
-      <c r="D20" s="112">
+      <c r="D20" s="93">
         <v>1089.92</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="109" t="s">
+      <c r="A21" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="110">
+      <c r="B21" s="91">
         <v>45658</v>
       </c>
-      <c r="C21" s="111">
+      <c r="C21" s="92">
         <v>8.59</v>
       </c>
-      <c r="D21" s="112">
+      <c r="D21" s="93">
         <v>1093.83</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="109" t="s">
+      <c r="A22" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="110">
+      <c r="B22" s="91">
         <v>46388</v>
       </c>
-      <c r="C22" s="111">
+      <c r="C22" s="92">
         <v>8.85</v>
       </c>
-      <c r="D22" s="112">
+      <c r="D22" s="93">
         <v>1094.97</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="109" t="s">
+      <c r="A23" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="110">
+      <c r="B23" s="91">
         <v>47119</v>
       </c>
-      <c r="C23" s="111">
+      <c r="C23" s="92">
         <v>8.9499999999999993</v>
       </c>
-      <c r="D23" s="112">
+      <c r="D23" s="93">
         <v>1099.56</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="107" t="s">
+      <c r="A24" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="108"/>
-      <c r="C24" s="108"/>
-      <c r="D24" s="108"/>
+      <c r="B24" s="115"/>
+      <c r="C24" s="115"/>
+      <c r="D24" s="115"/>
     </row>
     <row r="25" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="109" t="s">
+      <c r="A25" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="110">
+      <c r="B25" s="91">
         <v>44256</v>
       </c>
-      <c r="C25" s="111">
+      <c r="C25" s="92">
         <v>0.01</v>
       </c>
-      <c r="D25" s="112">
+      <c r="D25" s="93">
         <v>10092.549999999999</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="109" t="s">
+      <c r="A26" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="110">
+      <c r="B26" s="91">
         <v>44986</v>
       </c>
-      <c r="C26" s="111">
+      <c r="C26" s="92">
         <v>0.02</v>
       </c>
-      <c r="D26" s="112">
+      <c r="D26" s="93">
         <v>10086.68</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="109" t="s">
+      <c r="A27" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="110">
+      <c r="B27" s="91">
         <v>45717</v>
       </c>
-      <c r="C27" s="111">
+      <c r="C27" s="92">
         <v>0.03</v>
       </c>
-      <c r="D27" s="112">
+      <c r="D27" s="93">
         <v>10076.780000000001</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="107" t="s">
+      <c r="A28" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="108"/>
-      <c r="C28" s="108"/>
-      <c r="D28" s="108"/>
+      <c r="B28" s="115"/>
+      <c r="C28" s="115"/>
+      <c r="D28" s="115"/>
     </row>
     <row r="29" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="109" t="s">
+      <c r="A29" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="110">
+      <c r="B29" s="91">
         <v>44287</v>
       </c>
-      <c r="C29" s="111">
+      <c r="C29" s="92">
         <v>3.05</v>
       </c>
-      <c r="D29" s="112">
+      <c r="D29" s="93">
         <v>4205.83</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="109" t="s">
+      <c r="A30" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="B30" s="110">
+      <c r="B30" s="91">
         <v>47849</v>
       </c>
-      <c r="C30" s="111">
+      <c r="C30" s="92">
         <v>4.2699999999999996</v>
       </c>
-      <c r="D30" s="112">
+      <c r="D30" s="93">
         <v>6834.05</v>
       </c>
     </row>
@@ -6015,13 +6689,436 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="87" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="87" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="87" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="89" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="115"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="90" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="91">
+        <v>43600</v>
+      </c>
+      <c r="C3" s="92">
+        <v>-1.41</v>
+      </c>
+      <c r="D3" s="93">
+        <v>3222.98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="91">
+        <v>45519</v>
+      </c>
+      <c r="C4" s="92">
+        <v>4.16</v>
+      </c>
+      <c r="D4" s="93">
+        <v>2600.69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="90" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="91">
+        <v>49444</v>
+      </c>
+      <c r="C5" s="92">
+        <v>4.49</v>
+      </c>
+      <c r="D5" s="93">
+        <v>1597.97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="90" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="91">
+        <v>53097</v>
+      </c>
+      <c r="C6" s="92">
+        <v>4.49</v>
+      </c>
+      <c r="D6" s="93">
+        <v>1031.22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="91">
+        <v>44058</v>
+      </c>
+      <c r="C7" s="92">
+        <v>2.83</v>
+      </c>
+      <c r="D7" s="93">
+        <v>3389.02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="90" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="91">
+        <v>45519</v>
+      </c>
+      <c r="C8" s="92">
+        <v>4.09</v>
+      </c>
+      <c r="D8" s="93">
+        <v>3549.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="91">
+        <v>46249</v>
+      </c>
+      <c r="C9" s="92">
+        <v>4.18</v>
+      </c>
+      <c r="D9" s="93">
+        <v>3622.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="90" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="91">
+        <v>49444</v>
+      </c>
+      <c r="C10" s="92">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D10" s="93">
+        <v>3894.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="90" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="91">
+        <v>53097</v>
+      </c>
+      <c r="C11" s="92">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="D11" s="93">
+        <v>4031.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="91">
+        <v>55015</v>
+      </c>
+      <c r="C12" s="92">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="D12" s="93">
+        <v>4052.23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="89" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="115"/>
+      <c r="C13" s="115"/>
+      <c r="D13" s="115"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="90" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="91">
+        <v>43831</v>
+      </c>
+      <c r="C14" s="92">
+        <v>6.46</v>
+      </c>
+      <c r="D14" s="93">
+        <v>959.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="90" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="91">
+        <v>44197</v>
+      </c>
+      <c r="C15" s="92">
+        <v>7.09</v>
+      </c>
+      <c r="D15" s="93">
+        <v>892.83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="90" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="91">
+        <v>44562</v>
+      </c>
+      <c r="C16" s="92">
+        <v>7.78</v>
+      </c>
+      <c r="D16" s="93">
+        <v>819.87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="90" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="91">
+        <v>44927</v>
+      </c>
+      <c r="C17" s="92">
+        <v>8.24</v>
+      </c>
+      <c r="D17" s="93">
+        <v>749.19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="90" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="91">
+        <v>45658</v>
+      </c>
+      <c r="C18" s="92">
+        <v>8.75</v>
+      </c>
+      <c r="D18" s="93">
+        <v>622.91999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="90" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="91">
+        <v>44197</v>
+      </c>
+      <c r="C19" s="92">
+        <v>7.04</v>
+      </c>
+      <c r="D19" s="93">
+        <v>1077.29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="90" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="91">
+        <v>44927</v>
+      </c>
+      <c r="C20" s="92">
+        <v>8.1</v>
+      </c>
+      <c r="D20" s="93">
+        <v>1090.8800000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="90" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="91">
+        <v>45658</v>
+      </c>
+      <c r="C21" s="92">
+        <v>8.56</v>
+      </c>
+      <c r="D21" s="93">
+        <v>1095.51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="90" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="91">
+        <v>46388</v>
+      </c>
+      <c r="C22" s="92">
+        <v>8.82</v>
+      </c>
+      <c r="D22" s="93">
+        <v>1096.99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="90" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="91">
+        <v>47119</v>
+      </c>
+      <c r="C23" s="92">
+        <v>8.92</v>
+      </c>
+      <c r="D23" s="93">
+        <v>1101.8599999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="89" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="115"/>
+      <c r="C24" s="115"/>
+      <c r="D24" s="115"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="91">
+        <v>44256</v>
+      </c>
+      <c r="C25" s="92">
+        <v>0.01</v>
+      </c>
+      <c r="D25" s="93">
+        <v>10095.030000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="90" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="91">
+        <v>44986</v>
+      </c>
+      <c r="C26" s="92">
+        <v>0.02</v>
+      </c>
+      <c r="D26" s="93">
+        <v>10089.18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="91">
+        <v>45717</v>
+      </c>
+      <c r="C27" s="92">
+        <v>0.03</v>
+      </c>
+      <c r="D27" s="93">
+        <v>10079.27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="89" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="115"/>
+      <c r="C28" s="115"/>
+      <c r="D28" s="115"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="90" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="91">
+        <v>44287</v>
+      </c>
+      <c r="C29" s="92">
+        <v>3.06</v>
+      </c>
+      <c r="D29" s="93">
+        <v>4206.08</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="90" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="91">
+        <v>47849</v>
+      </c>
+      <c r="C30" s="92">
+        <v>4.26</v>
+      </c>
+      <c r="D30" s="93">
+        <v>6840.97</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B28:D28"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AG115"/>
   <sheetViews>
-    <sheetView topLeftCell="E25" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35:J37"/>
+    <sheetView topLeftCell="D18" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35:L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6062,41 +7159,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
-      <c r="K1" s="101"/>
-      <c r="L1" s="101"/>
-      <c r="M1" s="101"/>
-      <c r="N1" s="101"/>
-      <c r="O1" s="101"/>
-      <c r="P1" s="101"/>
-      <c r="Q1" s="101"/>
-      <c r="R1" s="101"/>
-      <c r="S1" s="101"/>
-      <c r="T1" s="101"/>
-      <c r="U1" s="101"/>
-      <c r="V1" s="101"/>
-      <c r="W1" s="101"/>
-      <c r="X1" s="101"/>
-      <c r="Y1" s="101"/>
-      <c r="Z1" s="101"/>
-      <c r="AA1" s="101"/>
-      <c r="AB1" s="101"/>
-      <c r="AC1" s="101"/>
-      <c r="AD1" s="101"/>
-      <c r="AE1" s="101"/>
-      <c r="AF1" s="101"/>
-      <c r="AG1" s="102"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="117"/>
+      <c r="G1" s="117"/>
+      <c r="H1" s="117"/>
+      <c r="I1" s="117"/>
+      <c r="J1" s="117"/>
+      <c r="K1" s="117"/>
+      <c r="L1" s="117"/>
+      <c r="M1" s="117"/>
+      <c r="N1" s="117"/>
+      <c r="O1" s="117"/>
+      <c r="P1" s="117"/>
+      <c r="Q1" s="117"/>
+      <c r="R1" s="117"/>
+      <c r="S1" s="117"/>
+      <c r="T1" s="117"/>
+      <c r="U1" s="117"/>
+      <c r="V1" s="117"/>
+      <c r="W1" s="117"/>
+      <c r="X1" s="117"/>
+      <c r="Y1" s="117"/>
+      <c r="Z1" s="117"/>
+      <c r="AA1" s="117"/>
+      <c r="AB1" s="117"/>
+      <c r="AC1" s="117"/>
+      <c r="AD1" s="117"/>
+      <c r="AE1" s="117"/>
+      <c r="AF1" s="117"/>
+      <c r="AG1" s="118"/>
     </row>
     <row r="2" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -6228,8 +7325,12 @@
       <c r="J3" s="15">
         <v>43592</v>
       </c>
-      <c r="K3" s="22"/>
-      <c r="L3" s="24"/>
+      <c r="K3" s="22">
+        <v>43593</v>
+      </c>
+      <c r="L3" s="24">
+        <v>43593</v>
+      </c>
       <c r="M3" s="22"/>
       <c r="N3" s="24"/>
       <c r="O3" s="22"/>
@@ -6277,14 +7378,18 @@
       <c r="H4" s="69">
         <v>3222.04</v>
       </c>
-      <c r="I4" s="113">
+      <c r="I4" s="94">
         <v>-1.38</v>
       </c>
-      <c r="J4" s="114">
+      <c r="J4" s="95">
         <v>3222.48</v>
       </c>
-      <c r="K4" s="56"/>
-      <c r="L4" s="57"/>
+      <c r="K4" s="94">
+        <v>-1.41</v>
+      </c>
+      <c r="L4" s="95">
+        <v>3222.98</v>
+      </c>
       <c r="M4" s="56"/>
       <c r="N4" s="57"/>
       <c r="O4" s="56"/>
@@ -6332,14 +7437,18 @@
       <c r="H5" s="61">
         <v>2598.79</v>
       </c>
-      <c r="I5" s="115">
+      <c r="I5" s="96">
         <v>4.16</v>
       </c>
-      <c r="J5" s="116">
+      <c r="J5" s="97">
         <v>2599.7399999999998</v>
       </c>
-      <c r="K5" s="56"/>
-      <c r="L5" s="57"/>
+      <c r="K5" s="96">
+        <v>4.16</v>
+      </c>
+      <c r="L5" s="97">
+        <v>2600.69</v>
+      </c>
       <c r="M5" s="56"/>
       <c r="N5" s="57"/>
       <c r="O5" s="56"/>
@@ -6387,14 +7496,18 @@
       <c r="H6" s="61">
         <v>1589.46</v>
       </c>
-      <c r="I6" s="115">
+      <c r="I6" s="96">
         <v>4.5</v>
       </c>
-      <c r="J6" s="116">
+      <c r="J6" s="97">
         <v>1594.93</v>
       </c>
-      <c r="K6" s="56"/>
-      <c r="L6" s="57"/>
+      <c r="K6" s="96">
+        <v>4.49</v>
+      </c>
+      <c r="L6" s="97">
+        <v>1597.97</v>
+      </c>
       <c r="M6" s="56"/>
       <c r="N6" s="57"/>
       <c r="O6" s="56"/>
@@ -6442,14 +7555,18 @@
       <c r="H7" s="61">
         <v>1022.79</v>
       </c>
-      <c r="I7" s="115">
+      <c r="I7" s="96">
         <v>4.5</v>
       </c>
-      <c r="J7" s="116">
+      <c r="J7" s="97">
         <v>1028.27</v>
       </c>
-      <c r="K7" s="56"/>
-      <c r="L7" s="57"/>
+      <c r="K7" s="96">
+        <v>4.49</v>
+      </c>
+      <c r="L7" s="97">
+        <v>1031.22</v>
+      </c>
       <c r="M7" s="56"/>
       <c r="N7" s="57"/>
       <c r="O7" s="56"/>
@@ -6497,14 +7614,18 @@
       <c r="H8" s="61">
         <v>3387.31</v>
       </c>
-      <c r="I8" s="115">
+      <c r="I8" s="96">
         <v>2.82</v>
       </c>
-      <c r="J8" s="116">
+      <c r="J8" s="97">
         <v>3388.37</v>
       </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="17"/>
+      <c r="K8" s="96">
+        <v>2.83</v>
+      </c>
+      <c r="L8" s="97">
+        <v>3389.02</v>
+      </c>
       <c r="M8" s="16"/>
       <c r="N8" s="17"/>
       <c r="O8" s="16"/>
@@ -6552,14 +7673,18 @@
       <c r="H9" s="61">
         <v>3546.94</v>
       </c>
-      <c r="I9" s="115">
+      <c r="I9" s="96">
         <v>4.09</v>
       </c>
-      <c r="J9" s="116">
+      <c r="J9" s="97">
         <v>3548.22</v>
       </c>
-      <c r="K9" s="16"/>
-      <c r="L9" s="17"/>
+      <c r="K9" s="96">
+        <v>4.09</v>
+      </c>
+      <c r="L9" s="97">
+        <v>3549.5</v>
+      </c>
       <c r="M9" s="16"/>
       <c r="N9" s="17"/>
       <c r="O9" s="16"/>
@@ -6607,14 +7732,18 @@
       <c r="H10" s="61">
         <v>3620.06</v>
       </c>
-      <c r="I10" s="115">
+      <c r="I10" s="96">
         <v>4.1900000000000004</v>
       </c>
-      <c r="J10" s="116">
+      <c r="J10" s="97">
         <v>3619.29</v>
       </c>
-      <c r="K10" s="16"/>
-      <c r="L10" s="17"/>
+      <c r="K10" s="96">
+        <v>4.18</v>
+      </c>
+      <c r="L10" s="97">
+        <v>3622.7</v>
+      </c>
       <c r="M10" s="16"/>
       <c r="N10" s="17"/>
       <c r="O10" s="16"/>
@@ -6662,14 +7791,18 @@
       <c r="H11" s="61">
         <v>3879.48</v>
       </c>
-      <c r="I11" s="115">
+      <c r="I11" s="96">
         <v>4.41</v>
       </c>
-      <c r="J11" s="116">
+      <c r="J11" s="97">
         <v>3888.93</v>
       </c>
-      <c r="K11" s="16"/>
-      <c r="L11" s="17"/>
+      <c r="K11" s="96">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="L11" s="97">
+        <v>3894.4</v>
+      </c>
       <c r="M11" s="16"/>
       <c r="N11" s="17"/>
       <c r="O11" s="16"/>
@@ -6717,14 +7850,18 @@
       <c r="H12" s="61">
         <v>4017.47</v>
       </c>
-      <c r="I12" s="115">
+      <c r="I12" s="96">
         <v>4.53</v>
       </c>
-      <c r="J12" s="116">
+      <c r="J12" s="97">
         <v>4024.53</v>
       </c>
-      <c r="K12" s="16"/>
-      <c r="L12" s="17"/>
+      <c r="K12" s="96">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="L12" s="97">
+        <v>4031.6</v>
+      </c>
       <c r="M12" s="16"/>
       <c r="N12" s="17"/>
       <c r="O12" s="16"/>
@@ -6772,14 +7909,18 @@
       <c r="H13" s="63">
         <v>4036.78</v>
       </c>
-      <c r="I13" s="117">
+      <c r="I13" s="98">
         <v>4.53</v>
       </c>
-      <c r="J13" s="118">
+      <c r="J13" s="99">
         <v>4044.5</v>
       </c>
-      <c r="K13" s="16"/>
-      <c r="L13" s="17"/>
+      <c r="K13" s="98">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="L13" s="99">
+        <v>4052.23</v>
+      </c>
       <c r="M13" s="16"/>
       <c r="N13" s="17"/>
       <c r="O13" s="16"/>
@@ -6803,41 +7944,41 @@
       <c r="AG13" s="17"/>
     </row>
     <row r="14" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="100" t="s">
+      <c r="A14" s="116" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="101"/>
-      <c r="C14" s="103"/>
-      <c r="D14" s="103"/>
-      <c r="E14" s="103"/>
-      <c r="F14" s="103"/>
-      <c r="G14" s="103"/>
-      <c r="H14" s="103"/>
-      <c r="I14" s="101"/>
-      <c r="J14" s="101"/>
-      <c r="K14" s="101"/>
-      <c r="L14" s="101"/>
-      <c r="M14" s="101"/>
-      <c r="N14" s="101"/>
-      <c r="O14" s="101"/>
-      <c r="P14" s="101"/>
-      <c r="Q14" s="101"/>
-      <c r="R14" s="101"/>
-      <c r="S14" s="101"/>
-      <c r="T14" s="101"/>
-      <c r="U14" s="101"/>
-      <c r="V14" s="101"/>
-      <c r="W14" s="101"/>
-      <c r="X14" s="101"/>
-      <c r="Y14" s="101"/>
-      <c r="Z14" s="101"/>
-      <c r="AA14" s="101"/>
-      <c r="AB14" s="101"/>
-      <c r="AC14" s="101"/>
-      <c r="AD14" s="101"/>
-      <c r="AE14" s="101"/>
-      <c r="AF14" s="101"/>
-      <c r="AG14" s="102"/>
+      <c r="B14" s="117"/>
+      <c r="C14" s="119"/>
+      <c r="D14" s="119"/>
+      <c r="E14" s="119"/>
+      <c r="F14" s="119"/>
+      <c r="G14" s="119"/>
+      <c r="H14" s="119"/>
+      <c r="I14" s="117"/>
+      <c r="J14" s="117"/>
+      <c r="K14" s="117"/>
+      <c r="L14" s="117"/>
+      <c r="M14" s="117"/>
+      <c r="N14" s="117"/>
+      <c r="O14" s="117"/>
+      <c r="P14" s="117"/>
+      <c r="Q14" s="117"/>
+      <c r="R14" s="117"/>
+      <c r="S14" s="117"/>
+      <c r="T14" s="117"/>
+      <c r="U14" s="117"/>
+      <c r="V14" s="117"/>
+      <c r="W14" s="117"/>
+      <c r="X14" s="117"/>
+      <c r="Y14" s="117"/>
+      <c r="Z14" s="117"/>
+      <c r="AA14" s="117"/>
+      <c r="AB14" s="117"/>
+      <c r="AC14" s="117"/>
+      <c r="AD14" s="117"/>
+      <c r="AE14" s="117"/>
+      <c r="AF14" s="117"/>
+      <c r="AG14" s="118"/>
     </row>
     <row r="15" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
@@ -6969,8 +8110,12 @@
       <c r="J16" s="4">
         <v>43592</v>
       </c>
-      <c r="K16" s="22"/>
-      <c r="L16" s="24"/>
+      <c r="K16" s="22">
+        <v>43593</v>
+      </c>
+      <c r="L16" s="24">
+        <v>43593</v>
+      </c>
       <c r="M16" s="22"/>
       <c r="N16" s="24"/>
       <c r="O16" s="22"/>
@@ -7018,14 +8163,18 @@
       <c r="H17" s="69">
         <v>958.76</v>
       </c>
-      <c r="I17" s="113">
+      <c r="I17" s="94">
         <v>6.48</v>
       </c>
-      <c r="J17" s="114">
+      <c r="J17" s="95">
         <v>959.24</v>
       </c>
-      <c r="K17" s="56"/>
-      <c r="L17" s="57"/>
+      <c r="K17" s="94">
+        <v>6.46</v>
+      </c>
+      <c r="L17" s="95">
+        <v>959.6</v>
+      </c>
       <c r="M17" s="56"/>
       <c r="N17" s="57"/>
       <c r="O17" s="56"/>
@@ -7073,14 +8222,18 @@
       <c r="H18" s="61">
         <v>891.66</v>
       </c>
-      <c r="I18" s="115">
+      <c r="I18" s="96">
         <v>7.11</v>
       </c>
-      <c r="J18" s="116">
+      <c r="J18" s="97">
         <v>892.31</v>
       </c>
-      <c r="K18" s="56"/>
-      <c r="L18" s="57"/>
+      <c r="K18" s="96">
+        <v>7.09</v>
+      </c>
+      <c r="L18" s="97">
+        <v>892.83</v>
+      </c>
       <c r="M18" s="56"/>
       <c r="N18" s="57"/>
       <c r="O18" s="56"/>
@@ -7128,14 +8281,18 @@
       <c r="H19" s="61">
         <v>818.78</v>
       </c>
-      <c r="I19" s="115">
+      <c r="I19" s="96">
         <v>7.79</v>
       </c>
-      <c r="J19" s="116">
+      <c r="J19" s="97">
         <v>819.43</v>
       </c>
-      <c r="K19" s="56"/>
-      <c r="L19" s="57"/>
+      <c r="K19" s="96">
+        <v>7.78</v>
+      </c>
+      <c r="L19" s="97">
+        <v>819.87</v>
+      </c>
       <c r="M19" s="56"/>
       <c r="N19" s="57"/>
       <c r="O19" s="56"/>
@@ -7183,14 +8340,18 @@
       <c r="H20" s="61">
         <v>748.21</v>
       </c>
-      <c r="I20" s="115">
+      <c r="I20" s="96">
         <v>8.25</v>
       </c>
-      <c r="J20" s="116">
+      <c r="J20" s="97">
         <v>748.7</v>
       </c>
-      <c r="K20" s="56"/>
-      <c r="L20" s="57"/>
+      <c r="K20" s="96">
+        <v>8.24</v>
+      </c>
+      <c r="L20" s="97">
+        <v>749.19</v>
+      </c>
       <c r="M20" s="56"/>
       <c r="N20" s="57"/>
       <c r="O20" s="56"/>
@@ -7238,14 +8399,18 @@
       <c r="H21" s="61">
         <v>621.21</v>
       </c>
-      <c r="I21" s="115">
+      <c r="I21" s="96">
         <v>8.77</v>
       </c>
-      <c r="J21" s="116">
+      <c r="J21" s="97">
         <v>622.07000000000005</v>
       </c>
-      <c r="K21" s="56"/>
-      <c r="L21" s="57"/>
+      <c r="K21" s="96">
+        <v>8.75</v>
+      </c>
+      <c r="L21" s="97">
+        <v>622.91999999999996</v>
+      </c>
       <c r="M21" s="56"/>
       <c r="N21" s="57"/>
       <c r="O21" s="56"/>
@@ -7293,14 +8458,18 @@
       <c r="H22" s="61">
         <v>1075.94</v>
       </c>
-      <c r="I22" s="115">
+      <c r="I22" s="96">
         <v>7.06</v>
       </c>
-      <c r="J22" s="116">
+      <c r="J22" s="97">
         <v>1076.69</v>
       </c>
-      <c r="K22" s="56"/>
-      <c r="L22" s="57"/>
+      <c r="K22" s="96">
+        <v>7.04</v>
+      </c>
+      <c r="L22" s="97">
+        <v>1077.29</v>
+      </c>
       <c r="M22" s="56"/>
       <c r="N22" s="57"/>
       <c r="O22" s="56"/>
@@ -7348,14 +8517,18 @@
       <c r="H23" s="61">
         <v>1089.27</v>
       </c>
-      <c r="I23" s="115">
+      <c r="I23" s="96">
         <v>8.1199999999999992</v>
       </c>
-      <c r="J23" s="116">
+      <c r="J23" s="97">
         <v>1089.92</v>
       </c>
-      <c r="K23" s="56"/>
-      <c r="L23" s="57"/>
+      <c r="K23" s="96">
+        <v>8.1</v>
+      </c>
+      <c r="L23" s="97">
+        <v>1090.8800000000001</v>
+      </c>
       <c r="M23" s="56"/>
       <c r="N23" s="57"/>
       <c r="O23" s="56"/>
@@ -7403,14 +8576,18 @@
       <c r="H24" s="61">
         <v>1092.5899999999999</v>
       </c>
-      <c r="I24" s="115">
+      <c r="I24" s="96">
         <v>8.59</v>
       </c>
-      <c r="J24" s="116">
+      <c r="J24" s="97">
         <v>1093.83</v>
       </c>
-      <c r="K24" s="16"/>
-      <c r="L24" s="17"/>
+      <c r="K24" s="96">
+        <v>8.56</v>
+      </c>
+      <c r="L24" s="97">
+        <v>1095.51</v>
+      </c>
       <c r="M24" s="16"/>
       <c r="N24" s="17"/>
       <c r="O24" s="16"/>
@@ -7458,14 +8635,18 @@
       <c r="H25" s="61">
         <v>1092.96</v>
       </c>
-      <c r="I25" s="115">
+      <c r="I25" s="96">
         <v>8.85</v>
       </c>
-      <c r="J25" s="116">
+      <c r="J25" s="97">
         <v>1094.97</v>
       </c>
-      <c r="K25" s="16"/>
-      <c r="L25" s="17"/>
+      <c r="K25" s="96">
+        <v>8.82</v>
+      </c>
+      <c r="L25" s="97">
+        <v>1096.99</v>
+      </c>
       <c r="M25" s="16"/>
       <c r="N25" s="17"/>
       <c r="O25" s="16"/>
@@ -7513,14 +8694,18 @@
       <c r="H26" s="63">
         <v>1096.6199999999999</v>
       </c>
-      <c r="I26" s="117">
+      <c r="I26" s="98">
         <v>8.9499999999999993</v>
       </c>
-      <c r="J26" s="118">
+      <c r="J26" s="99">
         <v>1099.56</v>
       </c>
-      <c r="K26" s="16"/>
-      <c r="L26" s="17"/>
+      <c r="K26" s="98">
+        <v>8.92</v>
+      </c>
+      <c r="L26" s="99">
+        <v>1101.8599999999999</v>
+      </c>
       <c r="M26" s="16"/>
       <c r="N26" s="17"/>
       <c r="O26" s="16"/>
@@ -7544,41 +8729,41 @@
       <c r="AG26" s="17"/>
     </row>
     <row r="27" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="100" t="s">
+      <c r="A27" s="116" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="101"/>
-      <c r="C27" s="103"/>
-      <c r="D27" s="103"/>
-      <c r="E27" s="103"/>
-      <c r="F27" s="103"/>
-      <c r="G27" s="103"/>
-      <c r="H27" s="103"/>
-      <c r="I27" s="101"/>
-      <c r="J27" s="101"/>
-      <c r="K27" s="101"/>
-      <c r="L27" s="101"/>
-      <c r="M27" s="101"/>
-      <c r="N27" s="101"/>
-      <c r="O27" s="101"/>
-      <c r="P27" s="101"/>
-      <c r="Q27" s="101"/>
-      <c r="R27" s="101"/>
-      <c r="S27" s="101"/>
-      <c r="T27" s="101"/>
-      <c r="U27" s="101"/>
-      <c r="V27" s="101"/>
-      <c r="W27" s="101"/>
-      <c r="X27" s="101"/>
-      <c r="Y27" s="101"/>
-      <c r="Z27" s="101"/>
-      <c r="AA27" s="101"/>
-      <c r="AB27" s="101"/>
-      <c r="AC27" s="101"/>
-      <c r="AD27" s="101"/>
-      <c r="AE27" s="101"/>
-      <c r="AF27" s="101"/>
-      <c r="AG27" s="102"/>
+      <c r="B27" s="117"/>
+      <c r="C27" s="119"/>
+      <c r="D27" s="119"/>
+      <c r="E27" s="119"/>
+      <c r="F27" s="119"/>
+      <c r="G27" s="119"/>
+      <c r="H27" s="119"/>
+      <c r="I27" s="117"/>
+      <c r="J27" s="117"/>
+      <c r="K27" s="117"/>
+      <c r="L27" s="117"/>
+      <c r="M27" s="117"/>
+      <c r="N27" s="117"/>
+      <c r="O27" s="117"/>
+      <c r="P27" s="117"/>
+      <c r="Q27" s="117"/>
+      <c r="R27" s="117"/>
+      <c r="S27" s="117"/>
+      <c r="T27" s="117"/>
+      <c r="U27" s="117"/>
+      <c r="V27" s="117"/>
+      <c r="W27" s="117"/>
+      <c r="X27" s="117"/>
+      <c r="Y27" s="117"/>
+      <c r="Z27" s="117"/>
+      <c r="AA27" s="117"/>
+      <c r="AB27" s="117"/>
+      <c r="AC27" s="117"/>
+      <c r="AD27" s="117"/>
+      <c r="AE27" s="117"/>
+      <c r="AF27" s="117"/>
+      <c r="AG27" s="118"/>
     </row>
     <row r="28" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="74" t="s">
@@ -7710,8 +8895,12 @@
       <c r="J29" s="4">
         <v>43592</v>
       </c>
-      <c r="K29" s="22"/>
-      <c r="L29" s="24"/>
+      <c r="K29" s="22">
+        <v>43593</v>
+      </c>
+      <c r="L29" s="24">
+        <v>43593</v>
+      </c>
       <c r="M29" s="22"/>
       <c r="N29" s="24"/>
       <c r="O29" s="22"/>
@@ -7759,14 +8948,18 @@
       <c r="H30" s="69">
         <v>10090.049999999999</v>
       </c>
-      <c r="I30" s="113">
+      <c r="I30" s="94">
         <v>0.01</v>
       </c>
-      <c r="J30" s="114">
+      <c r="J30" s="95">
         <v>10092.549999999999</v>
       </c>
-      <c r="K30" s="56"/>
-      <c r="L30" s="57"/>
+      <c r="K30" s="94">
+        <v>0.01</v>
+      </c>
+      <c r="L30" s="95">
+        <v>10095.030000000001</v>
+      </c>
       <c r="M30" s="56"/>
       <c r="N30" s="57"/>
       <c r="O30" s="56"/>
@@ -7814,14 +9007,18 @@
       <c r="H31" s="61">
         <v>10084.19</v>
       </c>
-      <c r="I31" s="115">
+      <c r="I31" s="96">
         <v>0.02</v>
       </c>
-      <c r="J31" s="116">
+      <c r="J31" s="97">
         <v>10086.68</v>
       </c>
-      <c r="K31" s="56"/>
-      <c r="L31" s="57"/>
+      <c r="K31" s="96">
+        <v>0.02</v>
+      </c>
+      <c r="L31" s="97">
+        <v>10089.18</v>
+      </c>
       <c r="M31" s="56"/>
       <c r="N31" s="57"/>
       <c r="O31" s="56"/>
@@ -7869,14 +9066,18 @@
       <c r="H32" s="63">
         <v>10074.290000000001</v>
       </c>
-      <c r="I32" s="117">
+      <c r="I32" s="98">
         <v>0.03</v>
       </c>
-      <c r="J32" s="118">
+      <c r="J32" s="99">
         <v>10076.780000000001</v>
       </c>
-      <c r="K32" s="11"/>
-      <c r="L32" s="13"/>
+      <c r="K32" s="98">
+        <v>0.03</v>
+      </c>
+      <c r="L32" s="99">
+        <v>10079.27</v>
+      </c>
       <c r="M32" s="11"/>
       <c r="N32" s="13"/>
       <c r="O32" s="11"/>
@@ -7899,21 +9100,23 @@
       <c r="AF32" s="11"/>
       <c r="AG32" s="13"/>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="119" t="s">
+    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="120" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="120"/>
-      <c r="C33" s="120"/>
-      <c r="D33" s="120"/>
-      <c r="E33" s="120"/>
-      <c r="F33" s="120"/>
-      <c r="G33" s="120"/>
-      <c r="H33" s="120"/>
-      <c r="I33" s="120"/>
+      <c r="B33" s="121"/>
+      <c r="C33" s="121"/>
+      <c r="D33" s="121"/>
+      <c r="E33" s="121"/>
+      <c r="F33" s="121"/>
+      <c r="G33" s="121"/>
+      <c r="H33" s="121"/>
+      <c r="I33" s="121"/>
       <c r="J33" s="121"/>
-    </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K33" s="121"/>
+      <c r="L33" s="122"/>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="31" t="s">
         <v>1</v>
       </c>
@@ -7944,8 +9147,14 @@
       <c r="J34" s="32" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K34" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="L34" s="32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>18</v>
       </c>
@@ -7974,8 +9183,14 @@
       <c r="J35" s="15">
         <v>43592</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K35" s="10">
+        <v>43593</v>
+      </c>
+      <c r="L35" s="15">
+        <v>43593</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="64" t="s">
         <v>38</v>
       </c>
@@ -8000,14 +9215,20 @@
       <c r="H36" s="69">
         <v>4204.09</v>
       </c>
-      <c r="I36" s="113">
+      <c r="I36" s="94">
         <v>3.05</v>
       </c>
-      <c r="J36" s="114">
+      <c r="J36" s="95">
         <v>4205.83</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K36" s="94">
+        <v>3.06</v>
+      </c>
+      <c r="L36" s="95">
+        <v>4206.08</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="66" t="s">
         <v>39</v>
       </c>
@@ -8032,24 +9253,30 @@
       <c r="H37" s="63">
         <v>6827.13</v>
       </c>
-      <c r="I37" s="117">
+      <c r="I37" s="98">
         <v>4.2699999999999996</v>
       </c>
-      <c r="J37" s="118">
+      <c r="J37" s="99">
         <v>6834.05</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="K37" s="98">
+        <v>4.26</v>
+      </c>
+      <c r="L37" s="99">
+        <v>6840.97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8122,19 +9349,19 @@
     <mergeCell ref="A1:AG1"/>
     <mergeCell ref="A27:AG27"/>
     <mergeCell ref="A14:AG14"/>
-    <mergeCell ref="A33:J33"/>
+    <mergeCell ref="A33:L33"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF101"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8170,40 +9397,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="123" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="103"/>
-      <c r="H1" s="103"/>
-      <c r="I1" s="103"/>
-      <c r="J1" s="103"/>
-      <c r="K1" s="103"/>
-      <c r="L1" s="103"/>
-      <c r="M1" s="103"/>
-      <c r="N1" s="103"/>
-      <c r="O1" s="103"/>
-      <c r="P1" s="103"/>
-      <c r="Q1" s="103"/>
-      <c r="R1" s="103"/>
-      <c r="S1" s="103"/>
-      <c r="T1" s="103"/>
-      <c r="U1" s="103"/>
-      <c r="V1" s="103"/>
-      <c r="W1" s="103"/>
-      <c r="X1" s="103"/>
-      <c r="Y1" s="103"/>
-      <c r="Z1" s="103"/>
-      <c r="AA1" s="103"/>
-      <c r="AB1" s="103"/>
-      <c r="AC1" s="103"/>
-      <c r="AD1" s="103"/>
-      <c r="AE1" s="103"/>
-      <c r="AF1" s="103"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="119"/>
+      <c r="P1" s="119"/>
+      <c r="Q1" s="119"/>
+      <c r="R1" s="119"/>
+      <c r="S1" s="119"/>
+      <c r="T1" s="119"/>
+      <c r="U1" s="119"/>
+      <c r="V1" s="119"/>
+      <c r="W1" s="119"/>
+      <c r="X1" s="119"/>
+      <c r="Y1" s="119"/>
+      <c r="Z1" s="119"/>
+      <c r="AA1" s="119"/>
+      <c r="AB1" s="119"/>
+      <c r="AC1" s="119"/>
+      <c r="AD1" s="119"/>
+      <c r="AE1" s="119"/>
+      <c r="AF1" s="119"/>
     </row>
     <row r="2" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
@@ -8332,8 +9559,12 @@
       <c r="J3" s="15">
         <v>43592</v>
       </c>
-      <c r="K3" s="22"/>
-      <c r="L3" s="24"/>
+      <c r="K3" s="22">
+        <v>43593</v>
+      </c>
+      <c r="L3" s="24">
+        <v>43593</v>
+      </c>
       <c r="M3" s="22"/>
       <c r="N3" s="24"/>
       <c r="O3" s="22"/>
@@ -8380,14 +9611,18 @@
       <c r="H4" s="69">
         <v>3222.04</v>
       </c>
-      <c r="I4" s="113">
+      <c r="I4" s="94">
         <v>-1.38</v>
       </c>
-      <c r="J4" s="114">
+      <c r="J4" s="95">
         <v>3222.48</v>
       </c>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
+      <c r="K4" s="94">
+        <v>-1.41</v>
+      </c>
+      <c r="L4" s="95">
+        <v>3222.98</v>
+      </c>
       <c r="M4" s="23"/>
       <c r="N4" s="23"/>
       <c r="O4" s="23"/>
@@ -8434,14 +9669,18 @@
       <c r="H5" s="61">
         <v>2598.79</v>
       </c>
-      <c r="I5" s="115">
+      <c r="I5" s="96">
         <v>4.16</v>
       </c>
-      <c r="J5" s="116">
+      <c r="J5" s="97">
         <v>2599.7399999999998</v>
       </c>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
+      <c r="K5" s="96">
+        <v>4.16</v>
+      </c>
+      <c r="L5" s="97">
+        <v>2600.69</v>
+      </c>
       <c r="M5" s="35"/>
       <c r="N5" s="35"/>
       <c r="O5" s="35"/>
@@ -8488,14 +9727,18 @@
       <c r="H6" s="61">
         <v>1589.46</v>
       </c>
-      <c r="I6" s="115">
+      <c r="I6" s="96">
         <v>4.5</v>
       </c>
-      <c r="J6" s="116">
+      <c r="J6" s="97">
         <v>1594.93</v>
       </c>
-      <c r="K6" s="80"/>
-      <c r="L6" s="8"/>
+      <c r="K6" s="96">
+        <v>4.49</v>
+      </c>
+      <c r="L6" s="97">
+        <v>1597.97</v>
+      </c>
       <c r="M6" s="80"/>
       <c r="N6" s="8"/>
       <c r="O6" s="80"/>
@@ -8542,14 +9785,18 @@
       <c r="H7" s="63">
         <v>1022.79</v>
       </c>
-      <c r="I7" s="117">
+      <c r="I7" s="98">
         <v>4.5</v>
       </c>
-      <c r="J7" s="118">
+      <c r="J7" s="99">
         <v>1028.27</v>
       </c>
-      <c r="K7" s="83"/>
-      <c r="L7" s="12"/>
+      <c r="K7" s="98">
+        <v>4.49</v>
+      </c>
+      <c r="L7" s="99">
+        <v>1031.22</v>
+      </c>
       <c r="M7" s="83"/>
       <c r="N7" s="12"/>
       <c r="O7" s="83"/>
@@ -8675,12 +9922,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF103"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J4" sqref="I4:J9"/>
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8700,40 +9947,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="124" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
-      <c r="Q1" s="105"/>
-      <c r="R1" s="105"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="105"/>
-      <c r="U1" s="105"/>
-      <c r="V1" s="105"/>
-      <c r="W1" s="105"/>
-      <c r="X1" s="105"/>
-      <c r="Y1" s="105"/>
-      <c r="Z1" s="105"/>
-      <c r="AA1" s="105"/>
-      <c r="AB1" s="105"/>
-      <c r="AC1" s="105"/>
-      <c r="AD1" s="105"/>
-      <c r="AE1" s="105"/>
-      <c r="AF1" s="105"/>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="124"/>
+      <c r="K1" s="124"/>
+      <c r="L1" s="124"/>
+      <c r="M1" s="124"/>
+      <c r="N1" s="124"/>
+      <c r="O1" s="124"/>
+      <c r="P1" s="124"/>
+      <c r="Q1" s="124"/>
+      <c r="R1" s="124"/>
+      <c r="S1" s="124"/>
+      <c r="T1" s="124"/>
+      <c r="U1" s="124"/>
+      <c r="V1" s="124"/>
+      <c r="W1" s="124"/>
+      <c r="X1" s="124"/>
+      <c r="Y1" s="124"/>
+      <c r="Z1" s="124"/>
+      <c r="AA1" s="124"/>
+      <c r="AB1" s="124"/>
+      <c r="AC1" s="124"/>
+      <c r="AD1" s="124"/>
+      <c r="AE1" s="124"/>
+      <c r="AF1" s="124"/>
     </row>
     <row r="2" spans="1:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -8862,8 +10109,12 @@
       <c r="J3" s="4">
         <v>43592</v>
       </c>
-      <c r="K3" s="22"/>
-      <c r="L3" s="23"/>
+      <c r="K3" s="22">
+        <v>43593</v>
+      </c>
+      <c r="L3" s="23">
+        <v>43593</v>
+      </c>
       <c r="M3" s="22"/>
       <c r="N3" s="24"/>
       <c r="O3" s="22"/>
@@ -8910,14 +10161,18 @@
       <c r="H4" s="69">
         <v>3387.31</v>
       </c>
-      <c r="I4" s="113">
+      <c r="I4" s="94">
         <v>2.82</v>
       </c>
-      <c r="J4" s="114">
+      <c r="J4" s="95">
         <v>3388.37</v>
       </c>
-      <c r="K4" s="56"/>
-      <c r="L4" s="35"/>
+      <c r="K4" s="94">
+        <v>2.83</v>
+      </c>
+      <c r="L4" s="95">
+        <v>3389.02</v>
+      </c>
       <c r="M4" s="56"/>
       <c r="N4" s="57"/>
       <c r="O4" s="56"/>
@@ -8964,14 +10219,18 @@
       <c r="H5" s="61">
         <v>3546.94</v>
       </c>
-      <c r="I5" s="115">
+      <c r="I5" s="96">
         <v>4.09</v>
       </c>
-      <c r="J5" s="116">
+      <c r="J5" s="97">
         <v>3548.22</v>
       </c>
-      <c r="K5" s="56"/>
-      <c r="L5" s="35"/>
+      <c r="K5" s="96">
+        <v>4.09</v>
+      </c>
+      <c r="L5" s="97">
+        <v>3549.5</v>
+      </c>
       <c r="M5" s="56"/>
       <c r="N5" s="57"/>
       <c r="O5" s="56"/>
@@ -9018,14 +10277,18 @@
       <c r="H6" s="61">
         <v>3620.06</v>
       </c>
-      <c r="I6" s="115">
+      <c r="I6" s="96">
         <v>4.1900000000000004</v>
       </c>
-      <c r="J6" s="116">
+      <c r="J6" s="97">
         <v>3619.29</v>
       </c>
-      <c r="K6" s="56"/>
-      <c r="L6" s="35"/>
+      <c r="K6" s="96">
+        <v>4.18</v>
+      </c>
+      <c r="L6" s="97">
+        <v>3622.7</v>
+      </c>
       <c r="M6" s="56"/>
       <c r="N6" s="57"/>
       <c r="O6" s="56"/>
@@ -9072,14 +10335,18 @@
       <c r="H7" s="61">
         <v>3879.48</v>
       </c>
-      <c r="I7" s="115">
+      <c r="I7" s="96">
         <v>4.41</v>
       </c>
-      <c r="J7" s="116">
+      <c r="J7" s="97">
         <v>3888.93</v>
       </c>
-      <c r="K7" s="16"/>
-      <c r="L7" s="8"/>
+      <c r="K7" s="96">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="L7" s="97">
+        <v>3894.4</v>
+      </c>
       <c r="M7" s="16"/>
       <c r="N7" s="17"/>
       <c r="O7" s="16"/>
@@ -9126,14 +10393,18 @@
       <c r="H8" s="61">
         <v>4017.47</v>
       </c>
-      <c r="I8" s="115">
+      <c r="I8" s="96">
         <v>4.53</v>
       </c>
-      <c r="J8" s="116">
+      <c r="J8" s="97">
         <v>4024.53</v>
       </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="8"/>
+      <c r="K8" s="96">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="L8" s="97">
+        <v>4031.6</v>
+      </c>
       <c r="M8" s="16"/>
       <c r="N8" s="17"/>
       <c r="O8" s="16"/>
@@ -9180,14 +10451,18 @@
       <c r="H9" s="63">
         <v>4036.78</v>
       </c>
-      <c r="I9" s="117">
+      <c r="I9" s="98">
         <v>4.53</v>
       </c>
-      <c r="J9" s="118">
+      <c r="J9" s="99">
         <v>4044.5</v>
       </c>
-      <c r="K9" s="11"/>
-      <c r="L9" s="12"/>
+      <c r="K9" s="98">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="L9" s="99">
+        <v>4052.23</v>
+      </c>
       <c r="M9" s="11"/>
       <c r="N9" s="13"/>
       <c r="O9" s="11"/>
@@ -9312,12 +10587,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG102"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:J8"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9337,40 +10612,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
-      <c r="Q1" s="105"/>
-      <c r="R1" s="105"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="105"/>
-      <c r="U1" s="105"/>
-      <c r="V1" s="105"/>
-      <c r="W1" s="105"/>
-      <c r="X1" s="105"/>
-      <c r="Y1" s="105"/>
-      <c r="Z1" s="105"/>
-      <c r="AA1" s="105"/>
-      <c r="AB1" s="105"/>
-      <c r="AC1" s="105"/>
-      <c r="AD1" s="105"/>
-      <c r="AE1" s="105"/>
-      <c r="AF1" s="105"/>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="124"/>
+      <c r="K1" s="124"/>
+      <c r="L1" s="124"/>
+      <c r="M1" s="124"/>
+      <c r="N1" s="124"/>
+      <c r="O1" s="124"/>
+      <c r="P1" s="124"/>
+      <c r="Q1" s="124"/>
+      <c r="R1" s="124"/>
+      <c r="S1" s="124"/>
+      <c r="T1" s="124"/>
+      <c r="U1" s="124"/>
+      <c r="V1" s="124"/>
+      <c r="W1" s="124"/>
+      <c r="X1" s="124"/>
+      <c r="Y1" s="124"/>
+      <c r="Z1" s="124"/>
+      <c r="AA1" s="124"/>
+      <c r="AB1" s="124"/>
+      <c r="AC1" s="124"/>
+      <c r="AD1" s="124"/>
+      <c r="AE1" s="124"/>
+      <c r="AF1" s="124"/>
     </row>
     <row r="2" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -9397,10 +10672,10 @@
       <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="122" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="122" t="s">
+      <c r="I2" s="100" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="100" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="29" t="s">
@@ -9499,8 +10774,12 @@
       <c r="J3" s="15">
         <v>43592</v>
       </c>
-      <c r="K3" s="22"/>
-      <c r="L3" s="24"/>
+      <c r="K3" s="22">
+        <v>43593</v>
+      </c>
+      <c r="L3" s="24">
+        <v>43593</v>
+      </c>
       <c r="M3" s="22"/>
       <c r="N3" s="24"/>
       <c r="O3" s="22"/>
@@ -9547,14 +10826,18 @@
       <c r="H4" s="86">
         <v>958.76</v>
       </c>
-      <c r="I4" s="113">
+      <c r="I4" s="94">
         <v>6.48</v>
       </c>
-      <c r="J4" s="114">
+      <c r="J4" s="95">
         <v>959.24</v>
       </c>
-      <c r="K4" s="56"/>
-      <c r="L4" s="57"/>
+      <c r="K4" s="94">
+        <v>6.46</v>
+      </c>
+      <c r="L4" s="95">
+        <v>959.6</v>
+      </c>
       <c r="M4" s="56"/>
       <c r="N4" s="57"/>
       <c r="O4" s="56"/>
@@ -9602,14 +10885,18 @@
       <c r="H5" s="59">
         <v>891.66</v>
       </c>
-      <c r="I5" s="115">
+      <c r="I5" s="96">
         <v>7.11</v>
       </c>
-      <c r="J5" s="116">
+      <c r="J5" s="97">
         <v>892.31</v>
       </c>
-      <c r="K5" s="56"/>
-      <c r="L5" s="57"/>
+      <c r="K5" s="96">
+        <v>7.09</v>
+      </c>
+      <c r="L5" s="97">
+        <v>892.83</v>
+      </c>
       <c r="M5" s="56"/>
       <c r="N5" s="57"/>
       <c r="O5" s="56"/>
@@ -9657,14 +10944,18 @@
       <c r="H6" s="59">
         <v>818.78</v>
       </c>
-      <c r="I6" s="115">
+      <c r="I6" s="96">
         <v>7.79</v>
       </c>
-      <c r="J6" s="116">
+      <c r="J6" s="97">
         <v>819.43</v>
       </c>
-      <c r="K6" s="56"/>
-      <c r="L6" s="57"/>
+      <c r="K6" s="96">
+        <v>7.78</v>
+      </c>
+      <c r="L6" s="97">
+        <v>819.87</v>
+      </c>
       <c r="M6" s="56"/>
       <c r="N6" s="57"/>
       <c r="O6" s="56"/>
@@ -9712,14 +11003,18 @@
       <c r="H7" s="59">
         <v>748.21</v>
       </c>
-      <c r="I7" s="115">
+      <c r="I7" s="96">
         <v>8.25</v>
       </c>
-      <c r="J7" s="116">
+      <c r="J7" s="97">
         <v>748.7</v>
       </c>
-      <c r="K7" s="56"/>
-      <c r="L7" s="57"/>
+      <c r="K7" s="96">
+        <v>8.24</v>
+      </c>
+      <c r="L7" s="97">
+        <v>749.19</v>
+      </c>
       <c r="M7" s="56"/>
       <c r="N7" s="57"/>
       <c r="O7" s="56"/>
@@ -9767,14 +11062,18 @@
       <c r="H8" s="70">
         <v>621.21</v>
       </c>
-      <c r="I8" s="117">
+      <c r="I8" s="98">
         <v>8.77</v>
       </c>
-      <c r="J8" s="118">
+      <c r="J8" s="99">
         <v>622.07000000000005</v>
       </c>
-      <c r="K8" s="56"/>
-      <c r="L8" s="57"/>
+      <c r="K8" s="98">
+        <v>8.75</v>
+      </c>
+      <c r="L8" s="99">
+        <v>622.91999999999996</v>
+      </c>
       <c r="M8" s="56"/>
       <c r="N8" s="57"/>
       <c r="O8" s="56"/>
@@ -9796,594 +11095,6 @@
       <c r="AE8" s="57"/>
       <c r="AF8" s="56"/>
       <c r="AG8" s="57"/>
-    </row>
-    <row r="9" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:AF1"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG102"/>
-  <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J4" sqref="I4:J8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="28.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="28.85546875" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" customWidth="1"/>
-    <col min="11" max="11" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="105" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="105"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="105"/>
-      <c r="M1" s="105"/>
-      <c r="N1" s="105"/>
-      <c r="O1" s="105"/>
-      <c r="P1" s="105"/>
-      <c r="Q1" s="105"/>
-      <c r="R1" s="105"/>
-      <c r="S1" s="105"/>
-      <c r="T1" s="105"/>
-      <c r="U1" s="105"/>
-      <c r="V1" s="105"/>
-      <c r="W1" s="105"/>
-      <c r="X1" s="105"/>
-      <c r="Y1" s="105"/>
-      <c r="Z1" s="105"/>
-      <c r="AA1" s="105"/>
-      <c r="AB1" s="105"/>
-      <c r="AC1" s="105"/>
-      <c r="AD1" s="105"/>
-      <c r="AE1" s="105"/>
-      <c r="AF1" s="105"/>
-    </row>
-    <row r="2" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="N2" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="P2" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="R2" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="S2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="T2" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="U2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="V2" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="W2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="X2" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z2" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="AB2" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC2" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD2" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE2" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF2" s="21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="4">
-        <v>43587</v>
-      </c>
-      <c r="D3" s="5">
-        <v>43587</v>
-      </c>
-      <c r="E3" s="3">
-        <v>43588</v>
-      </c>
-      <c r="F3" s="5">
-        <v>43588</v>
-      </c>
-      <c r="G3" s="3">
-        <v>43591</v>
-      </c>
-      <c r="H3" s="4">
-        <v>43591</v>
-      </c>
-      <c r="I3" s="3">
-        <v>43592</v>
-      </c>
-      <c r="J3" s="4">
-        <v>43592</v>
-      </c>
-      <c r="K3" s="22"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="22"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="22"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="22"/>
-      <c r="Z3" s="24"/>
-      <c r="AA3" s="22"/>
-      <c r="AB3" s="24"/>
-      <c r="AC3" s="22"/>
-      <c r="AD3" s="24"/>
-      <c r="AE3" s="22"/>
-      <c r="AF3" s="24"/>
-    </row>
-    <row r="4" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="65">
-        <v>44197</v>
-      </c>
-      <c r="C4" s="68">
-        <v>7.19</v>
-      </c>
-      <c r="D4" s="69">
-        <v>1073.81</v>
-      </c>
-      <c r="E4" s="68">
-        <v>7.13</v>
-      </c>
-      <c r="F4" s="69">
-        <v>1075.03</v>
-      </c>
-      <c r="G4" s="68">
-        <v>7.09</v>
-      </c>
-      <c r="H4" s="69">
-        <v>1075.94</v>
-      </c>
-      <c r="I4" s="113">
-        <v>7.06</v>
-      </c>
-      <c r="J4" s="114">
-        <v>1076.69</v>
-      </c>
-      <c r="K4" s="56"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="56"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="35"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="56"/>
-      <c r="U4" s="57"/>
-      <c r="V4" s="56"/>
-      <c r="W4" s="57"/>
-      <c r="X4" s="56"/>
-      <c r="Y4" s="57"/>
-      <c r="Z4" s="56"/>
-      <c r="AA4" s="57"/>
-      <c r="AB4" s="56"/>
-      <c r="AC4" s="35"/>
-      <c r="AD4" s="56"/>
-      <c r="AE4" s="57"/>
-      <c r="AF4" s="56"/>
-      <c r="AG4" s="57"/>
-    </row>
-    <row r="5" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="71" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="72">
-        <v>44927</v>
-      </c>
-      <c r="C5" s="60">
-        <v>8.24</v>
-      </c>
-      <c r="D5" s="61">
-        <v>1085.18</v>
-      </c>
-      <c r="E5" s="60">
-        <v>8.18</v>
-      </c>
-      <c r="F5" s="61">
-        <v>1087.3800000000001</v>
-      </c>
-      <c r="G5" s="60">
-        <v>8.1300000000000008</v>
-      </c>
-      <c r="H5" s="61">
-        <v>1089.27</v>
-      </c>
-      <c r="I5" s="115">
-        <v>8.1199999999999992</v>
-      </c>
-      <c r="J5" s="116">
-        <v>1089.92</v>
-      </c>
-      <c r="K5" s="56"/>
-      <c r="L5" s="57"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="57"/>
-      <c r="O5" s="56"/>
-      <c r="P5" s="57"/>
-      <c r="Q5" s="56"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="57"/>
-      <c r="T5" s="56"/>
-      <c r="U5" s="57"/>
-      <c r="V5" s="56"/>
-      <c r="W5" s="57"/>
-      <c r="X5" s="56"/>
-      <c r="Y5" s="57"/>
-      <c r="Z5" s="56"/>
-      <c r="AA5" s="57"/>
-      <c r="AB5" s="56"/>
-      <c r="AC5" s="35"/>
-      <c r="AD5" s="56"/>
-      <c r="AE5" s="57"/>
-      <c r="AF5" s="56"/>
-      <c r="AG5" s="57"/>
-    </row>
-    <row r="6" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="71" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="72">
-        <v>45658</v>
-      </c>
-      <c r="C6" s="60">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="D6" s="61">
-        <v>1087.92</v>
-      </c>
-      <c r="E6" s="60">
-        <v>8.66</v>
-      </c>
-      <c r="F6" s="61">
-        <v>1090.04</v>
-      </c>
-      <c r="G6" s="60">
-        <v>8.61</v>
-      </c>
-      <c r="H6" s="61">
-        <v>1092.5899999999999</v>
-      </c>
-      <c r="I6" s="115">
-        <v>8.59</v>
-      </c>
-      <c r="J6" s="116">
-        <v>1093.83</v>
-      </c>
-      <c r="K6" s="16"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="17"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="17"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="16"/>
-      <c r="AA6" s="17"/>
-      <c r="AB6" s="16"/>
-      <c r="AC6" s="8"/>
-      <c r="AD6" s="16"/>
-      <c r="AE6" s="17"/>
-      <c r="AF6" s="16"/>
-      <c r="AG6" s="17"/>
-    </row>
-    <row r="7" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="71" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="72">
-        <v>46388</v>
-      </c>
-      <c r="C7" s="60">
-        <v>8.99</v>
-      </c>
-      <c r="D7" s="61">
-        <v>1086.21</v>
-      </c>
-      <c r="E7" s="60">
-        <v>8.93</v>
-      </c>
-      <c r="F7" s="61">
-        <v>1089.8499999999999</v>
-      </c>
-      <c r="G7" s="60">
-        <v>8.8800000000000008</v>
-      </c>
-      <c r="H7" s="61">
-        <v>1092.96</v>
-      </c>
-      <c r="I7" s="115">
-        <v>8.85</v>
-      </c>
-      <c r="J7" s="116">
-        <v>1094.97</v>
-      </c>
-      <c r="K7" s="16"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="17"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="17"/>
-      <c r="X7" s="16"/>
-      <c r="Y7" s="17"/>
-      <c r="Z7" s="16"/>
-      <c r="AA7" s="17"/>
-      <c r="AB7" s="16"/>
-      <c r="AC7" s="8"/>
-      <c r="AD7" s="16"/>
-      <c r="AE7" s="17"/>
-      <c r="AF7" s="16"/>
-      <c r="AG7" s="17"/>
-    </row>
-    <row r="8" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="66" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="67">
-        <v>47119</v>
-      </c>
-      <c r="C8" s="62">
-        <v>9.08</v>
-      </c>
-      <c r="D8" s="63">
-        <v>1090.1400000000001</v>
-      </c>
-      <c r="E8" s="62">
-        <v>9.0299999999999994</v>
-      </c>
-      <c r="F8" s="63">
-        <v>1093.69</v>
-      </c>
-      <c r="G8" s="62">
-        <v>8.99</v>
-      </c>
-      <c r="H8" s="63">
-        <v>1096.6199999999999</v>
-      </c>
-      <c r="I8" s="117">
-        <v>8.9499999999999993</v>
-      </c>
-      <c r="J8" s="118">
-        <v>1099.56</v>
-      </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="17"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="17"/>
-      <c r="X8" s="16"/>
-      <c r="Y8" s="17"/>
-      <c r="Z8" s="16"/>
-      <c r="AA8" s="17"/>
-      <c r="AB8" s="16"/>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="16"/>
-      <c r="AE8" s="17"/>
-      <c r="AF8" s="16"/>
-      <c r="AG8" s="17"/>
     </row>
     <row r="9" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>